<commit_message>
updated calculations and figures for peer review
</commit_message>
<xml_diff>
--- a/1_calculation_scripts/1_6_nitrogen/results/mie_results_vle_visc_fluid.xlsx
+++ b/1_calculation_scripts/1_6_nitrogen/results/mie_results_vle_visc_fluid.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>lambda_r</t>
   </si>
@@ -77,7 +77,13 @@
     <t>tcondl_vle_model</t>
   </si>
   <si>
+    <t>tcondl_vle_model_ann</t>
+  </si>
+  <si>
     <t>speed_of_sound_liq_vle_model</t>
+  </si>
+  <si>
+    <t>tcondl_vle_model_vib</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
         <v>131.58113621994</v>
       </c>
       <c r="E2">
-        <v>4190653.325019464</v>
+        <v>4190653.325019454</v>
       </c>
       <c r="F2">
-        <v>11290.88849941579</v>
+        <v>11290.8884994158</v>
       </c>
       <c r="G2">
         <v>3.673729892411237</v>
@@ -500,13 +506,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -546,8 +552,14 @@
       <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>42.33275587884645</v>
       </c>
@@ -585,10 +597,16 @@
         <v>0.1307742265970717</v>
       </c>
       <c r="M2">
+        <v>0.1307741421265878</v>
+      </c>
+      <c r="N2">
         <v>1354.814953224774</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2">
+        <v>8.447048396248761E-08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>43.23424137914677</v>
       </c>
@@ -626,10 +644,16 @@
         <v>0.1297876561992176</v>
       </c>
       <c r="M3">
+        <v>0.1297875701094199</v>
+      </c>
+      <c r="N3">
         <v>1290.661322897515</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3">
+        <v>8.60897977908141E-08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>44.13572687944708</v>
       </c>
@@ -667,10 +691,16 @@
         <v>0.1289466780802478</v>
       </c>
       <c r="M4">
+        <v>0.1289465902663813</v>
+      </c>
+      <c r="N4">
         <v>1243.360576836033</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="O4">
+        <v>8.781386657182816E-08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>45.0372123797474</v>
       </c>
@@ -708,10 +738,16 @@
         <v>0.1282418825148702</v>
       </c>
       <c r="M5">
+        <v>0.1282417928647129</v>
+      </c>
+      <c r="N5">
         <v>1207.169440325773</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="O5">
+        <v>8.965015736627892E-08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>45.93869788004772</v>
       </c>
@@ -749,10 +785,16 @@
         <v>0.1276639897884893</v>
       </c>
       <c r="M6">
+        <v>0.1276638981818665</v>
+      </c>
+      <c r="N6">
         <v>1178.674728405966</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="O6">
+        <v>9.160662276624699E-08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>46.84018338034804</v>
       </c>
@@ -790,10 +832,16 @@
         <v>0.1272034761920159</v>
       </c>
       <c r="M7">
+        <v>0.1272033825002989</v>
+      </c>
+      <c r="N7">
         <v>1155.705323387783</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7">
+        <v>9.369171698670403E-08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>47.74166888064835</v>
       </c>
@@ -831,10 +879,16 @@
         <v>0.1268502865535216</v>
       </c>
       <c r="M8">
+        <v>0.1268501906391132</v>
+      </c>
+      <c r="N8">
         <v>1136.804337140874</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8">
+        <v>9.591440845632641E-08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>48.64315438094867</v>
       </c>
@@ -872,10 +926,16 @@
         <v>0.1265936644599049</v>
       </c>
       <c r="M9">
+        <v>0.1265935661757168</v>
+      </c>
+      <c r="N9">
         <v>1120.950583460161</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9">
+        <v>9.828418813234387E-08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>49.54463988124898</v>
       </c>
@@ -913,10 +973,16 @@
         <v>0.1264221171070153</v>
       </c>
       <c r="M10">
+        <v>0.1264220162959427</v>
+      </c>
+      <c r="N10">
         <v>1107.401769396712</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10">
+        <v>1.008110726392579E-07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>50.4461253815493</v>
       </c>
@@ -954,10 +1020,16 @@
         <v>0.126323514856958</v>
       </c>
       <c r="M11">
+        <v>0.1263234113513568</v>
+      </c>
+      <c r="N11">
         <v>1095.601611445087</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11">
+        <v>1.035056012674966E-07</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>51.34761088184962</v>
       </c>
@@ -995,10 +1067,16 @@
         <v>0.1262853089678015</v>
       </c>
       <c r="M12">
+        <v>0.1262852025889758</v>
+      </c>
+      <c r="N12">
         <v>1085.122565748849</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="O12">
+        <v>1.063788257736451E-07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>52.24909638214994</v>
       </c>
@@ -1036,10 +1114,16 @@
         <v>0.1262948373933352</v>
       </c>
       <c r="M13">
+        <v>0.1262947279510433</v>
+      </c>
+      <c r="N13">
         <v>1075.629379713574</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13">
+        <v>1.09442291875392E-07</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>53.15058188245025</v>
       </c>
@@ -1077,10 +1161,16 @@
         <v>0.1263396800976912</v>
       </c>
       <c r="M14">
+        <v>0.1263395673896799</v>
+      </c>
+      <c r="N14">
         <v>1066.85529809435</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="O14">
+        <v>1.127080113098348E-07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>54.05206738275056</v>
       </c>
@@ -1118,10 +1208,16 @@
         <v>0.1264080226913861</v>
       </c>
       <c r="M15">
+        <v>0.1264079065029627</v>
+      </c>
+      <c r="N15">
         <v>1058.586189865994</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="O15">
+        <v>1.161884233410972E-07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>54.95355288305088</v>
       </c>
@@ -1159,59 +1255,71 @@
         <v>0.1264889898268227</v>
       </c>
       <c r="M16">
+        <v>0.126488869930478</v>
+      </c>
+      <c r="N16">
         <v>1050.649729515618</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16">
+        <v>1.198963446713281E-07</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
-        <v>55.85503838335121</v>
+        <v>55.85503838335119</v>
       </c>
       <c r="B17">
-        <v>3016.346978823382</v>
+        <v>3016.346978823406</v>
       </c>
       <c r="C17">
-        <v>6.513116489435649</v>
+        <v>6.513116489435703</v>
       </c>
       <c r="D17">
-        <v>31128.77369058563</v>
+        <v>31128.77369058562</v>
       </c>
       <c r="E17">
-        <v>6281.039317303702</v>
+        <v>6281.039317303703</v>
       </c>
       <c r="F17">
-        <v>5818.01737239155</v>
+        <v>5818.017372391548</v>
       </c>
       <c r="G17">
-        <v>24.19718631950125</v>
+        <v>24.19718631950128</v>
       </c>
       <c r="H17">
         <v>60.88342983327271</v>
       </c>
       <c r="I17">
-        <v>2.108937275500559E-09</v>
+        <v>2.108937275500564E-09</v>
       </c>
       <c r="J17">
-        <v>9.081531576335392E-10</v>
+        <v>9.081531576335394E-10</v>
       </c>
       <c r="K17">
-        <v>0.0005443735320955666</v>
+        <v>0.0005443735320955659</v>
       </c>
       <c r="L17">
         <v>0.126572916381339</v>
       </c>
       <c r="M17">
-        <v>1042.90782908152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>0.1265727925364321</v>
+      </c>
+      <c r="N17">
+        <v>1042.907829081519</v>
+      </c>
+      <c r="O17">
+        <v>1.238449068411843E-07</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>56.75652388365152</v>
       </c>
       <c r="B18">
-        <v>3738.337877559034</v>
+        <v>3738.337877559047</v>
       </c>
       <c r="C18">
-        <v>7.948057020533393</v>
+        <v>7.948057020533421</v>
       </c>
       <c r="D18">
         <v>30927.97351230042</v>
@@ -1241,18 +1349,24 @@
         <v>0.1266515334984442</v>
       </c>
       <c r="M18">
+        <v>0.1266514054509638</v>
+      </c>
+      <c r="N18">
         <v>1035.251150712357</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18">
+        <v>1.280474804009781E-07</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>57.65800938395183</v>
       </c>
       <c r="B19">
-        <v>4594.751305844394</v>
+        <v>4594.751305844398</v>
       </c>
       <c r="C19">
-        <v>9.621869388378688</v>
+        <v>9.621869388378695</v>
       </c>
       <c r="D19">
         <v>30733.30684439881</v>
@@ -1282,18 +1396,24 @@
         <v>0.1267180567217598</v>
       </c>
       <c r="M19">
+        <v>0.1267179242041744</v>
+      </c>
+      <c r="N19">
         <v>1027.5949266042</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="O19">
+        <v>1.32517585412095E-07</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>58.55949488425215</v>
       </c>
       <c r="B20">
-        <v>5603.479302015287</v>
+        <v>5603.479302015292</v>
       </c>
       <c r="C20">
-        <v>11.56136892271359</v>
+        <v>11.5613689227136</v>
       </c>
       <c r="D20">
         <v>30544.27768294936</v>
@@ -1323,18 +1443,24 @@
         <v>0.1267671736716378</v>
       </c>
       <c r="M20">
+        <v>0.1267670364028496</v>
+      </c>
+      <c r="N20">
         <v>1019.87557567173</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="O20">
+        <v>1.372687881889299E-07</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21">
-        <v>59.46098038455248</v>
+        <v>59.46098038455246</v>
       </c>
       <c r="B21">
-        <v>6783.79734056246</v>
+        <v>6783.797340562496</v>
       </c>
       <c r="C21">
-        <v>13.7948321804146</v>
+        <v>13.79483218041467</v>
       </c>
       <c r="D21">
         <v>30360.42656254468</v>
@@ -1343,39 +1469,45 @@
         <v>6083.438667246864</v>
       </c>
       <c r="F21">
-        <v>5591.898436406872</v>
+        <v>5591.898436406871</v>
       </c>
       <c r="G21">
-        <v>17.97290703696573</v>
+        <v>17.97290703696572</v>
       </c>
       <c r="H21">
-        <v>47.58169194407516</v>
+        <v>47.58169194407518</v>
       </c>
       <c r="I21">
-        <v>2.27097634087885E-09</v>
+        <v>2.270976340878851E-09</v>
       </c>
       <c r="J21">
-        <v>1.070001776376662E-09</v>
+        <v>1.070001776376661E-09</v>
       </c>
       <c r="K21">
-        <v>0.0004235092419477156</v>
+        <v>0.0004235092419477162</v>
       </c>
       <c r="L21">
         <v>0.1267949380903813</v>
       </c>
       <c r="M21">
+        <v>0.1267947957757967</v>
+      </c>
+      <c r="N21">
         <v>1012.047788460679</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="O21">
+        <v>1.423145846259076E-07</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>60.36246588485279</v>
       </c>
       <c r="B22">
-        <v>8156.374375511997</v>
+        <v>8156.374375511985</v>
       </c>
       <c r="C22">
-        <v>16.35196477939172</v>
+        <v>16.3519647793917</v>
       </c>
       <c r="D22">
         <v>30181.32728952333</v>
@@ -1405,15 +1537,21 @@
         <v>0.1267985848340674</v>
       </c>
       <c r="M22">
+        <v>0.1267984371657965</v>
+      </c>
+      <c r="N22">
         <v>1004.08188232163</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="O22">
+        <v>1.476682709530846E-07</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>61.2639513851531</v>
       </c>
       <c r="B23">
-        <v>9743.276664898905</v>
+        <v>9743.276664898907</v>
       </c>
       <c r="C23">
         <v>19.26386714881903</v>
@@ -1446,21 +1584,27 @@
         <v>0.1267762858814453</v>
       </c>
       <c r="M23">
+        <v>0.126776132538642</v>
+      </c>
+      <c r="N23">
         <v>995.9613227886969</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="O23">
+        <v>1.533428033268436E-07</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>62.16543688545342</v>
       </c>
       <c r="B24">
-        <v>11567.9655859608</v>
+        <v>11567.96558596065</v>
       </c>
       <c r="C24">
-        <v>22.5629991621259</v>
+        <v>22.56299916212561</v>
       </c>
       <c r="D24">
-        <v>29835.82843866862</v>
+        <v>29835.82843866863</v>
       </c>
       <c r="E24">
         <v>5960.587494492387</v>
@@ -1469,118 +1613,136 @@
         <v>5448.278941754149</v>
       </c>
       <c r="G24">
-        <v>14.68136513042085</v>
+        <v>14.68136513042083</v>
       </c>
       <c r="H24">
-        <v>40.53685875412248</v>
+        <v>40.53685875412244</v>
       </c>
       <c r="I24">
-        <v>2.407907499687003E-09</v>
+        <v>2.407907499687002E-09</v>
       </c>
       <c r="J24">
-        <v>1.219154343724628E-09</v>
+        <v>1.219154343724627E-09</v>
       </c>
       <c r="K24">
-        <v>0.0003493952505993937</v>
+        <v>0.0003493952505993939</v>
       </c>
       <c r="L24">
-        <v>0.1267268703057346</v>
+        <v>0.1267268703057347</v>
       </c>
       <c r="M24">
-        <v>987.6803725637424</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>0.1267267109550864</v>
+      </c>
+      <c r="N24">
+        <v>987.6803725637428</v>
+      </c>
+      <c r="O24">
+        <v>1.593506482542981E-07</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25">
-        <v>63.06692238575374</v>
+        <v>63.06692238575373</v>
       </c>
       <c r="B25">
-        <v>13655.2897103024</v>
+        <v>13655.28971030237</v>
       </c>
       <c r="C25">
-        <v>26.28314458891495</v>
+        <v>26.2831445889149</v>
       </c>
       <c r="D25">
-        <v>29668.71763843955</v>
+        <v>29668.71763843956</v>
       </c>
       <c r="E25">
-        <v>5923.15792028039</v>
+        <v>5923.157920280398</v>
       </c>
       <c r="F25">
-        <v>5404.07267101022</v>
+        <v>5404.072671010225</v>
       </c>
       <c r="G25">
-        <v>13.80356956036085</v>
+        <v>13.80356956036084</v>
       </c>
       <c r="H25">
-        <v>38.63888582630924</v>
+        <v>38.63888582630925</v>
       </c>
       <c r="I25">
         <v>2.457050770847755E-09</v>
       </c>
       <c r="J25">
-        <v>1.274900213893761E-09</v>
+        <v>1.274900213893758E-09</v>
       </c>
       <c r="K25">
-        <v>0.0003285548659557439</v>
+        <v>0.0003285548659557443</v>
       </c>
       <c r="L25">
-        <v>0.1266495314451273</v>
+        <v>0.1266495314451272</v>
       </c>
       <c r="M25">
-        <v>979.2418715804392</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>0.1266493657415008</v>
+      </c>
+      <c r="N25">
+        <v>979.2418715804395</v>
+      </c>
+      <c r="O25">
+        <v>1.657036264592227E-07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26">
-        <v>63.96840788605405</v>
+        <v>63.96840788605404</v>
       </c>
       <c r="B26">
-        <v>16031.47145901856</v>
+        <v>16031.47145901843</v>
       </c>
       <c r="C26">
-        <v>30.45937626148085</v>
+        <v>30.4593762614806</v>
       </c>
       <c r="D26">
         <v>29504.93162395737</v>
       </c>
       <c r="E26">
-        <v>5887.14515340184</v>
+        <v>5887.145153401842</v>
       </c>
       <c r="F26">
-        <v>5361.365463966853</v>
+        <v>5361.365463966858</v>
       </c>
       <c r="G26">
-        <v>13.02053306501903</v>
+        <v>13.02053306501908</v>
       </c>
       <c r="H26">
-        <v>36.93533819306769</v>
+        <v>36.93533819306775</v>
       </c>
       <c r="I26">
-        <v>2.508133697366461E-09</v>
+        <v>2.508133697366457E-09</v>
       </c>
       <c r="J26">
-        <v>1.333882976455729E-09</v>
+        <v>1.333882976455727E-09</v>
       </c>
       <c r="K26">
-        <v>0.0003095597035078061</v>
+        <v>0.0003095597035078069</v>
       </c>
       <c r="L26">
-        <v>0.1265435426338121</v>
+        <v>0.1265435426338122</v>
       </c>
       <c r="M26">
-        <v>970.6551744541529</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>0.1265433702210588</v>
+      </c>
+      <c r="N26">
+        <v>970.6551744541533</v>
+      </c>
+      <c r="O26">
+        <v>1.72412753373602E-07</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>64.86989338635436</v>
       </c>
       <c r="B27">
-        <v>18724.08869913027</v>
+        <v>18724.08869913049</v>
       </c>
       <c r="C27">
-        <v>35.12802280303773</v>
+        <v>35.12802280303814</v>
       </c>
       <c r="D27">
         <v>29344.17146555787</v>
@@ -1610,10 +1772,16 @@
         <v>0.1264079995011791</v>
       </c>
       <c r="M27">
+        <v>0.1264078200130992</v>
+      </c>
+      <c r="N27">
         <v>961.9342793327708</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="O27">
+        <v>1.794880799666493E-07</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28">
         <v>65.77137888665469</v>
       </c>
@@ -1651,59 +1819,71 @@
         <v>0.1262416027601669</v>
       </c>
       <c r="M28">
+        <v>0.1262414158216289</v>
+      </c>
+      <c r="N28">
         <v>953.0961790106871</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="O28">
+        <v>1.869385380297001E-07</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29">
-        <v>66.67286438695501</v>
+        <v>66.672864386955</v>
       </c>
       <c r="B29">
-        <v>25175.57568829246</v>
+        <v>25175.57568829238</v>
       </c>
       <c r="C29">
-        <v>46.09397152797765</v>
+        <v>46.09397152797751</v>
       </c>
       <c r="D29">
         <v>29030.62743631101</v>
       </c>
       <c r="E29">
-        <v>5785.852707263803</v>
+        <v>5785.852707263802</v>
       </c>
       <c r="F29">
-        <v>5240.540558610089</v>
+        <v>5240.54055861009</v>
       </c>
       <c r="G29">
-        <v>11.15494500679807</v>
+        <v>11.15494500679809</v>
       </c>
       <c r="H29">
-        <v>32.82990183957465</v>
+        <v>32.82990183957468</v>
       </c>
       <c r="I29">
-        <v>2.674260828347158E-09</v>
+        <v>2.674260828347156E-09</v>
       </c>
       <c r="J29">
         <v>1.531484447632598E-09</v>
       </c>
       <c r="K29">
-        <v>0.0002623509560350171</v>
+        <v>0.0002623509560350175</v>
       </c>
       <c r="L29">
         <v>0.126042491213039</v>
       </c>
       <c r="M29">
-        <v>944.1594553098478</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>0.1260422964412447</v>
+      </c>
+      <c r="N29">
+        <v>944.159455309848</v>
+      </c>
+      <c r="O29">
+        <v>1.947717943254319E-07</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30">
-        <v>67.57434988725532</v>
+        <v>67.57434988725531</v>
       </c>
       <c r="B30">
-        <v>28996.14996425775</v>
+        <v>28996.14996425771</v>
       </c>
       <c r="C30">
-        <v>52.46994778665317</v>
+        <v>52.46994778665312</v>
       </c>
       <c r="D30">
         <v>28877.33531890653</v>
@@ -1715,10 +1895,10 @@
         <v>5202.199908259612</v>
       </c>
       <c r="G30">
-        <v>10.66814771987703</v>
+        <v>10.66814771987704</v>
       </c>
       <c r="H30">
-        <v>31.74870172359493</v>
+        <v>31.74870172359499</v>
       </c>
       <c r="I30">
         <v>2.734374684100427E-09</v>
@@ -1727,24 +1907,30 @@
         <v>1.60460921491747E-09</v>
       </c>
       <c r="K30">
-        <v>0.0002493861578537831</v>
+        <v>0.000249386157853783</v>
       </c>
       <c r="L30">
         <v>0.1258081308027673</v>
       </c>
       <c r="M30">
-        <v>935.1431248514691</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>0.1258079278086492</v>
+      </c>
+      <c r="N30">
+        <v>935.1431248514693</v>
+      </c>
+      <c r="O30">
+        <v>2.029941181042493E-07</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31">
         <v>68.47583538755563</v>
       </c>
       <c r="B31">
-        <v>33256.50312834483</v>
+        <v>33256.50312834484</v>
       </c>
       <c r="C31">
-        <v>59.49564333510814</v>
+        <v>59.49564333510816</v>
       </c>
       <c r="D31">
         <v>28726.04966828966</v>
@@ -1774,18 +1960,24 @@
         <v>0.1255352620933243</v>
       </c>
       <c r="M31">
+        <v>0.1255350504830579</v>
+      </c>
+      <c r="N31">
         <v>926.0657313434283</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="O31">
+        <v>2.116102664094137E-07</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32">
         <v>69.37732088785596</v>
       </c>
       <c r="B32">
-        <v>37990.5657415344</v>
+        <v>37990.56574153443</v>
       </c>
       <c r="C32">
-        <v>67.21327362520184</v>
+        <v>67.21327362520188</v>
       </c>
       <c r="D32">
         <v>28576.55245082486</v>
@@ -1815,15 +2007,21 @@
         <v>0.1252199055711568</v>
       </c>
       <c r="M32">
+        <v>0.1252196849477655</v>
+      </c>
+      <c r="N32">
         <v>916.9446683669597</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="O32">
+        <v>2.206233912726278E-07</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>70.27880638815627</v>
       </c>
       <c r="B33">
-        <v>43233.430316071</v>
+        <v>43233.43031607099</v>
       </c>
       <c r="C33">
         <v>75.66618347634002</v>
@@ -1832,121 +2030,139 @@
         <v>28428.63786682472</v>
       </c>
       <c r="E33">
-        <v>5661.068837841653</v>
+        <v>5661.068837841652</v>
       </c>
       <c r="F33">
         <v>5091.219039097497</v>
       </c>
       <c r="G33">
-        <v>9.51815633026011</v>
+        <v>9.51815633026008</v>
       </c>
       <c r="H33">
-        <v>29.19836544992943</v>
+        <v>29.19836544992942</v>
       </c>
       <c r="I33">
-        <v>2.93102133104197E-09</v>
+        <v>2.931021331041969E-09</v>
       </c>
       <c r="J33">
-        <v>1.847058860382903E-09</v>
+        <v>1.847058860382901E-09</v>
       </c>
       <c r="K33">
-        <v>0.0002168695695550051</v>
+        <v>0.0002168695695550053</v>
       </c>
       <c r="L33">
         <v>0.1248574215684139</v>
       </c>
       <c r="M33">
-        <v>907.7957084318938</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>0.1248571915334415</v>
+      </c>
+      <c r="N33">
+        <v>907.7957084318942</v>
+      </c>
+      <c r="O33">
+        <v>2.300349724078373E-07</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34">
         <v>71.18029188845658</v>
       </c>
       <c r="B34">
-        <v>49021.30923162045</v>
+        <v>49021.30923162038</v>
       </c>
       <c r="C34">
-        <v>84.89884379853062</v>
+        <v>84.89884379853052</v>
       </c>
       <c r="D34">
-        <v>28282.11127927807</v>
+        <v>28282.11127927808</v>
       </c>
       <c r="E34">
-        <v>5630.895033170217</v>
+        <v>5630.895033170215</v>
       </c>
       <c r="F34">
-        <v>5055.219887292687</v>
+        <v>5055.21988729269</v>
       </c>
       <c r="G34">
-        <v>9.219368343859539</v>
+        <v>9.219368343859498</v>
       </c>
       <c r="H34">
-        <v>28.5462404482169</v>
+        <v>28.54624044821687</v>
       </c>
       <c r="I34">
-        <v>3.002566462627508E-09</v>
+        <v>3.002566462627497E-09</v>
       </c>
       <c r="J34">
-        <v>1.9358038388014E-09</v>
+        <v>1.935803838801395E-09</v>
       </c>
       <c r="K34">
-        <v>0.0002077682699850002</v>
+        <v>0.0002077682699850007</v>
       </c>
       <c r="L34">
-        <v>0.1244426194140738</v>
+        <v>0.1244426194140739</v>
       </c>
       <c r="M34">
-        <v>898.6327090942482</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+        <v>0.1244423795692956</v>
+      </c>
+      <c r="N34">
+        <v>898.6327090942501</v>
+      </c>
+      <c r="O34">
+        <v>2.398447782866539E-07</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35">
         <v>72.08177738875689</v>
       </c>
       <c r="B35">
-        <v>55391.49095336536</v>
+        <v>55391.49095336504</v>
       </c>
       <c r="C35">
-        <v>94.95685472413102</v>
+        <v>94.95685472413047</v>
       </c>
       <c r="D35">
         <v>28136.78822613398</v>
       </c>
       <c r="E35">
-        <v>5600.927458989197</v>
+        <v>5600.92745898919</v>
       </c>
       <c r="F35">
-        <v>5019.562856168196</v>
+        <v>5019.56285616819</v>
       </c>
       <c r="G35">
         <v>8.954693426137069</v>
       </c>
       <c r="H35">
-        <v>27.97891157840014</v>
+        <v>27.97891157840015</v>
       </c>
       <c r="I35">
-        <v>3.077418791272155E-09</v>
+        <v>3.077418791272158E-09</v>
       </c>
       <c r="J35">
-        <v>2.028601368482815E-09</v>
+        <v>2.028601368482817E-09</v>
       </c>
       <c r="K35">
-        <v>0.0001993730477687005</v>
+        <v>0.0001993730477687004</v>
       </c>
       <c r="L35">
         <v>0.1239699087360879</v>
       </c>
       <c r="M35">
-        <v>889.4674649640793</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+        <v>0.1239696586852302</v>
+      </c>
+      <c r="N35">
+        <v>889.467464964079</v>
+      </c>
+      <c r="O35">
+        <v>2.50050857624554E-07</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36">
         <v>72.98326288905722</v>
       </c>
       <c r="B36">
-        <v>62382.29493532245</v>
+        <v>62382.29493532243</v>
       </c>
       <c r="C36">
         <v>105.886955577155</v>
@@ -1979,15 +2195,21 @@
         <v>0.1234334848933942</v>
       </c>
       <c r="M36">
+        <v>0.1234332242438319</v>
+      </c>
+      <c r="N36">
         <v>880.3096749251064</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="O36">
+        <v>2.60649562316464E-07</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37">
-        <v>73.88474838935754</v>
+        <v>73.88474838935753</v>
       </c>
       <c r="B37">
-        <v>70033.02557138944</v>
+        <v>70033.02557138941</v>
       </c>
       <c r="C37">
         <v>117.7370420992542</v>
@@ -1999,80 +2221,92 @@
         <v>5541.264501767303</v>
       </c>
       <c r="F37">
-        <v>4948.953477234389</v>
+        <v>4948.95347723439</v>
       </c>
       <c r="G37">
-        <v>8.511443841723878</v>
+        <v>8.511443841723908</v>
       </c>
       <c r="H37">
-        <v>27.07040633091504</v>
+        <v>27.07040633091509</v>
       </c>
       <c r="I37">
-        <v>3.237879918730644E-09</v>
+        <v>3.237879918730642E-09</v>
       </c>
       <c r="J37">
         <v>2.226480916574707E-09</v>
       </c>
       <c r="K37">
-        <v>0.0001843910115603806</v>
+        <v>0.0001843910115603807</v>
       </c>
       <c r="L37">
         <v>0.1228275405715044</v>
       </c>
       <c r="M37">
-        <v>871.1669961625473</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>0.1228272689359026</v>
+      </c>
+      <c r="N37">
+        <v>871.1669961625475</v>
+      </c>
+      <c r="O37">
+        <v>2.71635601816829E-07</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38">
-        <v>74.78623388965785</v>
+        <v>74.78623388965784</v>
       </c>
       <c r="B38">
-        <v>78383.92553483712</v>
+        <v>78383.92553483696</v>
       </c>
       <c r="C38">
-        <v>130.5561913547327</v>
+        <v>130.5561913547324</v>
       </c>
       <c r="D38">
         <v>27706.32957496199</v>
       </c>
       <c r="E38">
-        <v>5511.411097557887</v>
+        <v>5511.411097557896</v>
       </c>
       <c r="F38">
-        <v>4913.855604809027</v>
+        <v>4913.855604809033</v>
       </c>
       <c r="G38">
-        <v>8.325812451769011</v>
+        <v>8.325812451768977</v>
       </c>
       <c r="H38">
-        <v>26.71693598055172</v>
+        <v>26.71693598055173</v>
       </c>
       <c r="I38">
-        <v>3.323944850987472E-09</v>
+        <v>3.323944850987477E-09</v>
       </c>
       <c r="J38">
-        <v>2.331597059992785E-09</v>
+        <v>2.331597059992787E-09</v>
       </c>
       <c r="K38">
-        <v>0.0001776736007140311</v>
+        <v>0.0001776736007140309</v>
       </c>
       <c r="L38">
         <v>0.1221464967711776</v>
       </c>
       <c r="M38">
+        <v>0.1221462137690496</v>
+      </c>
+      <c r="N38">
         <v>862.0451599808434</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="O38">
+        <v>2.830021279156958E-07</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39">
         <v>75.68771938995816</v>
       </c>
       <c r="B39">
-        <v>87476.12882454602</v>
+        <v>87476.12882454606</v>
       </c>
       <c r="C39">
-        <v>144.3946947537563</v>
+        <v>144.3946947537564</v>
       </c>
       <c r="D39">
         <v>27564.14896060032</v>
@@ -2102,182 +2336,212 @@
         <v>0.1213852485863133</v>
       </c>
       <c r="M39">
+        <v>0.1213849538454654</v>
+      </c>
+      <c r="N39">
         <v>852.9481283122904</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="O39">
+        <v>2.94740847864305E-07</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40">
         <v>76.58920489025849</v>
       </c>
       <c r="B40">
-        <v>97351.61381442517</v>
+        <v>97351.6138144252</v>
       </c>
       <c r="C40">
-        <v>159.3040996654516</v>
+        <v>159.3040996654517</v>
       </c>
       <c r="D40">
-        <v>27422.37246774168</v>
+        <v>27422.37246774167</v>
       </c>
       <c r="E40">
         <v>5451.304759434144</v>
       </c>
       <c r="F40">
-        <v>4843.749324686809</v>
+        <v>4843.749324686808</v>
       </c>
       <c r="G40">
         <v>8.011725771299881</v>
       </c>
       <c r="H40">
-        <v>26.18566097056851</v>
+        <v>26.1856609705685</v>
       </c>
       <c r="I40">
-        <v>3.509016467170771E-09</v>
+        <v>3.509016467170774E-09</v>
       </c>
       <c r="J40">
-        <v>2.554187000516285E-09</v>
+        <v>2.554187000516289E-09</v>
       </c>
       <c r="K40">
-        <v>0.0001655200023857136</v>
+        <v>0.0001655200023857135</v>
       </c>
       <c r="L40">
-        <v>0.1205394236444067</v>
+        <v>0.1205394236444066</v>
       </c>
       <c r="M40">
-        <v>843.8782738241441</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
+        <v>0.1205391168022437</v>
+      </c>
+      <c r="N40">
+        <v>843.8782738241438</v>
+      </c>
+      <c r="O40">
+        <v>3.068421629357911E-07</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41">
-        <v>77.49069039055881</v>
+        <v>77.4906903905588</v>
       </c>
       <c r="B41">
-        <v>108053.1565813723</v>
+        <v>108053.1565813721</v>
       </c>
       <c r="C41">
-        <v>175.3372601416374</v>
+        <v>175.337260141637</v>
       </c>
       <c r="D41">
         <v>27280.85964740448</v>
       </c>
       <c r="E41">
-        <v>5420.92304435691</v>
+        <v>5420.923044356912</v>
       </c>
       <c r="F41">
-        <v>4808.624858100778</v>
+        <v>4808.624858100779</v>
       </c>
       <c r="G41">
-        <v>7.878339415783424</v>
+        <v>7.878339415783483</v>
       </c>
       <c r="H41">
-        <v>25.99919760864287</v>
+        <v>25.99919760864294</v>
       </c>
       <c r="I41">
-        <v>3.608592968103125E-09</v>
+        <v>3.608592968103133E-09</v>
       </c>
       <c r="J41">
-        <v>2.671634934661292E-09</v>
+        <v>2.671634934661294E-09</v>
       </c>
       <c r="K41">
         <v>0.0001599971299569217</v>
       </c>
       <c r="L41">
-        <v>0.1196056526494756</v>
+        <v>0.1196056526494755</v>
       </c>
       <c r="M41">
-        <v>834.8365703164827</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>0.1196053333541467</v>
+      </c>
+      <c r="N41">
+        <v>834.8365703164815</v>
+      </c>
+      <c r="O41">
+        <v>3.192953287765812E-07</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42">
-        <v>78.39217589085912</v>
+        <v>78.39217589085911</v>
       </c>
       <c r="B42">
-        <v>119624.2847677485</v>
+        <v>119624.2847677472</v>
       </c>
       <c r="C42">
-        <v>192.5483973397941</v>
+        <v>192.5483973397919</v>
       </c>
       <c r="D42">
         <v>27139.47503219524</v>
       </c>
       <c r="E42">
-        <v>5390.242817550626</v>
+        <v>5390.242817550628</v>
       </c>
       <c r="F42">
-        <v>4773.38191743668</v>
+        <v>4773.381917436683</v>
       </c>
       <c r="G42">
-        <v>7.757915740608737</v>
+        <v>7.75791574060873</v>
       </c>
       <c r="H42">
         <v>25.86057220522226</v>
       </c>
       <c r="I42">
-        <v>3.713281589492533E-09</v>
+        <v>3.71328158949253E-09</v>
       </c>
       <c r="J42">
-        <v>2.793155201025733E-09</v>
+        <v>2.79315520102573E-09</v>
       </c>
       <c r="K42">
-        <v>0.0001547945831059656</v>
+        <v>0.0001547945831059658</v>
       </c>
       <c r="L42">
         <v>0.1185818504905693</v>
       </c>
       <c r="M42">
-        <v>825.8227834776804</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>0.118581518401936</v>
+      </c>
+      <c r="N42">
+        <v>825.8227834776808</v>
+      </c>
+      <c r="O42">
+        <v>3.320886333769149E-07</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43">
         <v>79.29366139115943</v>
       </c>
       <c r="B43">
-        <v>132109.2322170058</v>
+        <v>132109.2322170053</v>
       </c>
       <c r="C43">
-        <v>210.9931703222657</v>
+        <v>210.9931703222649</v>
       </c>
       <c r="D43">
         <v>26998.08757168573</v>
       </c>
       <c r="E43">
-        <v>5359.20860372995</v>
+        <v>5359.208603729952</v>
       </c>
       <c r="F43">
         <v>4737.971512880934</v>
       </c>
       <c r="G43">
-        <v>7.648663988185925</v>
+        <v>7.648663988185937</v>
       </c>
       <c r="H43">
-        <v>25.76662977109658</v>
+        <v>25.76662977109659</v>
       </c>
       <c r="I43">
-        <v>3.823428421970345E-09</v>
+        <v>3.823428421970346E-09</v>
       </c>
       <c r="J43">
-        <v>2.918718577953265E-09</v>
+        <v>2.918718577953263E-09</v>
       </c>
       <c r="K43">
-        <v>0.0001498811506932055</v>
+        <v>0.0001498811506932056</v>
       </c>
       <c r="L43">
-        <v>0.1174675012892704</v>
+        <v>0.1174675012892705</v>
       </c>
       <c r="M43">
-        <v>816.8356549375267</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>0.1174671560796823</v>
+      </c>
+      <c r="N43">
+        <v>816.8356549375263</v>
+      </c>
+      <c r="O43">
+        <v>3.452095881573982E-07</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44">
         <v>80.19514689145976</v>
       </c>
       <c r="B44">
-        <v>145552.8946063799</v>
+        <v>145552.8946063797</v>
       </c>
       <c r="C44">
-        <v>230.7287580200905</v>
+        <v>230.7287580200902</v>
       </c>
       <c r="D44">
         <v>26856.57009878817</v>
@@ -2307,36 +2571,42 @@
         <v>0.1162639308685545</v>
       </c>
       <c r="M44">
+        <v>0.1162635722234269</v>
+      </c>
+      <c r="N44">
         <v>807.8730749098853</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="O44">
+        <v>3.586451275577626E-07</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45">
-        <v>81.09663239176008</v>
+        <v>81.09663239176007</v>
       </c>
       <c r="B45">
-        <v>160000.7862888122</v>
+        <v>160000.7862888123</v>
       </c>
       <c r="C45">
-        <v>251.813953286896</v>
+        <v>251.8139532868961</v>
       </c>
       <c r="D45">
         <v>26714.79882364913</v>
       </c>
       <c r="E45">
-        <v>5295.870158362604</v>
+        <v>5295.870158362603</v>
       </c>
       <c r="F45">
         <v>4666.466524235821</v>
       </c>
       <c r="G45">
-        <v>7.457593102686183</v>
+        <v>7.457593102686255</v>
       </c>
       <c r="H45">
-        <v>25.70211269000257</v>
+        <v>25.70211269000264</v>
       </c>
       <c r="I45">
-        <v>4.061629322913399E-09</v>
+        <v>4.0616293229134E-09</v>
       </c>
       <c r="J45">
         <v>3.181841792473871E-09</v>
@@ -2348,68 +2618,80 @@
         <v>0.1149745366120694</v>
       </c>
       <c r="M45">
-        <v>798.932240573129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+        <v>0.1149741642302568</v>
+      </c>
+      <c r="N45">
+        <v>798.9322405731283</v>
+      </c>
+      <c r="O45">
+        <v>3.723818125807958E-07</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46">
-        <v>81.99811789206039</v>
+        <v>81.99811789206038</v>
       </c>
       <c r="B46">
-        <v>175498.9985480632</v>
+        <v>175498.998548063</v>
       </c>
       <c r="C46">
-        <v>274.309270134441</v>
+        <v>274.3092701344406</v>
       </c>
       <c r="D46">
         <v>26572.65285187235</v>
       </c>
       <c r="E46">
-        <v>5263.467778614168</v>
+        <v>5263.467778614166</v>
       </c>
       <c r="F46">
-        <v>4630.287121654862</v>
+        <v>4630.287121654861</v>
       </c>
       <c r="G46">
-        <v>7.373202340997004</v>
+        <v>7.373202340997008</v>
       </c>
       <c r="H46">
         <v>25.72706421611379</v>
       </c>
       <c r="I46">
-        <v>4.190533137411665E-09</v>
+        <v>4.190533137411663E-09</v>
       </c>
       <c r="J46">
-        <v>3.319332665721636E-09</v>
+        <v>3.31933266572163E-09</v>
       </c>
       <c r="K46">
-        <v>0.0001366155850471768</v>
+        <v>0.000136615585047177</v>
       </c>
       <c r="L46">
-        <v>0.113604931291187</v>
+        <v>0.1136049312911871</v>
       </c>
       <c r="M46">
-        <v>790.0097987507228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <v>0.1136045448851531</v>
+      </c>
+      <c r="N46">
+        <v>790.0097987507229</v>
+      </c>
+      <c r="O46">
+        <v>3.86406034006044E-07</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47">
         <v>82.8996033923607</v>
       </c>
       <c r="B47">
-        <v>192094.1594663439</v>
+        <v>192094.1594663411</v>
       </c>
       <c r="C47">
-        <v>298.2770654397556</v>
+        <v>298.2770654397507</v>
       </c>
       <c r="D47">
         <v>26430.01372413523</v>
       </c>
       <c r="E47">
-        <v>5230.51447678148</v>
+        <v>5230.514476781487</v>
       </c>
       <c r="F47">
-        <v>4593.770004913555</v>
+        <v>4593.770004913561</v>
       </c>
       <c r="G47">
         <v>7.294798417292598</v>
@@ -2430,59 +2712,71 @@
         <v>0.1121629502036147</v>
       </c>
       <c r="M47">
+        <v>0.1121625494994033</v>
+      </c>
+      <c r="N47">
         <v>781.1019724918044</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="O47">
+        <v>4.007042113706824E-07</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48">
         <v>83.80108889266101</v>
       </c>
       <c r="B48">
-        <v>209833.3956036244</v>
+        <v>209833.3956036246</v>
       </c>
       <c r="C48">
-        <v>323.781676649632</v>
+        <v>323.7816766496322</v>
       </c>
       <c r="D48">
         <v>26286.76497448916</v>
       </c>
       <c r="E48">
-        <v>5196.965657251523</v>
+        <v>5196.965657251525</v>
       </c>
       <c r="F48">
         <v>4556.877499058297</v>
       </c>
       <c r="G48">
-        <v>7.221474822869994</v>
+        <v>7.221474822870007</v>
       </c>
       <c r="H48">
-        <v>25.88249403584807</v>
+        <v>25.88249403584812</v>
       </c>
       <c r="I48">
-        <v>4.470360064475836E-09</v>
+        <v>4.470360064475846E-09</v>
       </c>
       <c r="J48">
-        <v>3.60601260058377E-09</v>
+        <v>3.606012600583771E-09</v>
       </c>
       <c r="K48">
-        <v>0.0001287895012825541</v>
+        <v>0.000128789501282554</v>
       </c>
       <c r="L48">
         <v>0.1106584764191875</v>
       </c>
       <c r="M48">
-        <v>772.2046718801142</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+        <v>0.1106580611562031</v>
+      </c>
+      <c r="N48">
+        <v>772.2046718801137</v>
+      </c>
+      <c r="O48">
+        <v>4.152629843163244E-07</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49">
-        <v>84.70257439296134</v>
+        <v>84.70257439296132</v>
       </c>
       <c r="B49">
         <v>228764.2956917625</v>
       </c>
       <c r="C49">
-        <v>350.8895772853115</v>
+        <v>350.8895772853116</v>
       </c>
       <c r="D49">
         <v>26142.79170483188</v>
@@ -2491,57 +2785,63 @@
         <v>5162.778006539337</v>
       </c>
       <c r="F49">
-        <v>4519.573343482504</v>
+        <v>4519.573343482502</v>
       </c>
       <c r="G49">
-        <v>7.152445903179965</v>
+        <v>7.152445903179946</v>
       </c>
       <c r="H49">
         <v>26.0102265795956</v>
       </c>
       <c r="I49">
-        <v>4.622381112926446E-09</v>
+        <v>4.622381112926451E-09</v>
       </c>
       <c r="J49">
-        <v>3.755150227294719E-09</v>
+        <v>3.755150227294721E-09</v>
       </c>
       <c r="K49">
-        <v>0.0001251301139153044</v>
+        <v>0.0001251301139153043</v>
       </c>
       <c r="L49">
-        <v>0.1091030609082603</v>
+        <v>0.1091030609082602</v>
       </c>
       <c r="M49">
+        <v>0.1091026308388667</v>
+      </c>
+      <c r="N49">
         <v>763.3135898831454</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="O49">
+        <v>4.300693934546613E-07</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50">
-        <v>85.60405989326165</v>
+        <v>85.60405989326163</v>
       </c>
       <c r="B50">
-        <v>248934.8765554619</v>
+        <v>248934.8765554618</v>
       </c>
       <c r="C50">
-        <v>379.6695523749544</v>
+        <v>379.6695523749542</v>
       </c>
       <c r="D50">
         <v>25997.980173214</v>
       </c>
       <c r="E50">
-        <v>5127.909231898541</v>
+        <v>5127.909231898547</v>
       </c>
       <c r="F50">
-        <v>4481.822450692126</v>
+        <v>4481.822450692129</v>
       </c>
       <c r="G50">
-        <v>7.087032449759226</v>
+        <v>7.087032449759207</v>
       </c>
       <c r="H50">
-        <v>26.16987592188565</v>
+        <v>26.16987592188567</v>
       </c>
       <c r="I50">
-        <v>4.783291103287165E-09</v>
+        <v>4.783291103287173E-09</v>
       </c>
       <c r="J50">
         <v>3.908130020245076E-09</v>
@@ -2550,30 +2850,36 @@
         <v>0.000121621131750908</v>
       </c>
       <c r="L50">
-        <v>0.1075093507702163</v>
+        <v>0.1075093507702164</v>
       </c>
       <c r="M50">
-        <v>754.4242843484658</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>0.1075089056591678</v>
+      </c>
+      <c r="N50">
+        <v>754.4242843484654</v>
+      </c>
+      <c r="O50">
+        <v>4.451110485102866E-07</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51">
         <v>86.50554539356196</v>
       </c>
       <c r="B51">
-        <v>270393.5514861482</v>
+        <v>270393.5514861485</v>
       </c>
       <c r="C51">
-        <v>410.1928963204444</v>
+        <v>410.1928963204448</v>
       </c>
       <c r="D51">
         <v>25852.21739379504</v>
       </c>
       <c r="E51">
-        <v>5092.317809450583</v>
+        <v>5092.317809450581</v>
       </c>
       <c r="F51">
-        <v>4443.590677147504</v>
+        <v>4443.590677147503</v>
       </c>
       <c r="G51">
         <v>7.024648874405504</v>
@@ -2594,18 +2900,24 @@
         <v>0.1058903805970934</v>
       </c>
       <c r="M51">
+        <v>0.1058899202208114</v>
+      </c>
+      <c r="N51">
         <v>745.5322474087387</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="O51">
+        <v>4.603762820594313E-07</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52">
-        <v>87.40703089386228</v>
+        <v>87.40703089386227</v>
       </c>
       <c r="B52">
-        <v>293189.1013138058</v>
+        <v>293189.1013138056</v>
       </c>
       <c r="C52">
-        <v>442.5336361446717</v>
+        <v>442.5336361446714</v>
       </c>
       <c r="D52">
         <v>25705.39074639704</v>
@@ -2614,13 +2926,13 @@
         <v>5055.962738910835</v>
       </c>
       <c r="F52">
-        <v>4404.844603475506</v>
+        <v>4404.844603475507</v>
       </c>
       <c r="G52">
-        <v>6.964791836803863</v>
+        <v>6.964791836803862</v>
       </c>
       <c r="H52">
-        <v>26.58194826199974</v>
+        <v>26.58194826199973</v>
       </c>
       <c r="I52">
         <v>5.134585646421054E-09</v>
@@ -2635,77 +2947,89 @@
         <v>0.1042588156926643</v>
       </c>
       <c r="M52">
+        <v>0.1042583398383766</v>
+      </c>
+      <c r="N52">
         <v>736.6329636099944</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="O52">
+        <v>4.758542877651183E-07</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53">
-        <v>88.30851639416261</v>
+        <v>88.30851639416258</v>
       </c>
       <c r="B53">
-        <v>317370.6484467381</v>
+        <v>317370.6484467434</v>
       </c>
       <c r="C53">
-        <v>476.7687835755731</v>
+        <v>476.768783575582</v>
       </c>
       <c r="D53">
         <v>25557.38759371885</v>
       </c>
       <c r="E53">
-        <v>5018.803302049255</v>
+        <v>5018.803302049254</v>
       </c>
       <c r="F53">
-        <v>4365.551321418848</v>
+        <v>4365.551321418846</v>
       </c>
       <c r="G53">
-        <v>6.907030199241977</v>
+        <v>6.907030199241976</v>
       </c>
       <c r="H53">
         <v>26.83338166977707</v>
       </c>
       <c r="I53">
-        <v>5.326546519247061E-09</v>
+        <v>5.326546519247062E-09</v>
       </c>
       <c r="J53">
-        <v>4.3901186554954E-09</v>
+        <v>4.390118655495399E-09</v>
       </c>
       <c r="K53">
         <v>0.0001118813815013361</v>
       </c>
       <c r="L53">
-        <v>0.102626249231758</v>
+        <v>0.1026262492317581</v>
       </c>
       <c r="M53">
-        <v>727.7219580601717</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+        <v>0.1026257576965156</v>
+      </c>
+      <c r="N53">
+        <v>727.7219580601716</v>
+      </c>
+      <c r="O53">
+        <v>4.915352424902552E-07</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54">
-        <v>89.21000189446292</v>
+        <v>89.21000189446291</v>
       </c>
       <c r="B54">
-        <v>342987.6341795749</v>
+        <v>342987.6341795741</v>
       </c>
       <c r="C54">
-        <v>512.9786200124092</v>
+        <v>512.9786200124081</v>
       </c>
       <c r="D54">
         <v>25408.09490437222</v>
       </c>
       <c r="E54">
-        <v>4980.798822065335</v>
+        <v>4980.798822065334</v>
       </c>
       <c r="F54">
         <v>4325.678224942612</v>
       </c>
       <c r="G54">
-        <v>6.850996186797644</v>
+        <v>6.85099618679765</v>
       </c>
       <c r="H54">
-        <v>27.11473261008764</v>
+        <v>27.11473261008762</v>
       </c>
       <c r="I54">
-        <v>5.530565207167264E-09</v>
+        <v>5.530565207167261E-09</v>
       </c>
       <c r="J54">
         <v>4.558524722891971E-09</v>
@@ -2717,10 +3041,16 @@
         <v>0.1010026434779162</v>
       </c>
       <c r="M54">
+        <v>0.1010021360675041</v>
+      </c>
+      <c r="N54">
         <v>718.7948358305451</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="O54">
+        <v>5.074104121196616E-07</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55">
         <v>90.11148739476323</v>
       </c>
@@ -2758,77 +3088,89 @@
         <v>0.09939597244311248</v>
       </c>
       <c r="M55">
+        <v>0.0993954489708712</v>
+      </c>
+      <c r="N55">
         <v>709.8473137490309</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="O55">
+        <v>5.234722412773177E-07</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56">
-        <v>91.01297289506356</v>
+        <v>91.01297289506354</v>
       </c>
       <c r="B56">
-        <v>398727.1705156389</v>
+        <v>398727.170515635</v>
       </c>
       <c r="C56">
-        <v>591.6618124174807</v>
+        <v>591.6618124174744</v>
       </c>
       <c r="D56">
-        <v>25105.18458465117</v>
+        <v>25105.18458465118</v>
       </c>
       <c r="E56">
-        <v>4902.090772975056</v>
+        <v>4902.090772975066</v>
       </c>
       <c r="F56">
-        <v>4244.062431085485</v>
+        <v>4244.062431085493</v>
       </c>
       <c r="G56">
-        <v>6.742911235845375</v>
+        <v>6.742911235845355</v>
       </c>
       <c r="H56">
-        <v>27.76721054688895</v>
+        <v>27.76721054688889</v>
       </c>
       <c r="I56">
-        <v>5.978875520277258E-09</v>
+        <v>5.978875520277247E-09</v>
       </c>
       <c r="J56">
-        <v>4.907214631202379E-09</v>
+        <v>4.907214631202371E-09</v>
       </c>
       <c r="K56">
         <v>0.0001031282191318294</v>
       </c>
       <c r="L56">
-        <v>0.09781208148586663</v>
+        <v>0.09781208148586672</v>
       </c>
       <c r="M56">
-        <v>700.875245614627</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+        <v>0.09781154177143932</v>
+      </c>
+      <c r="N56">
+        <v>700.8752456146275</v>
+      </c>
+      <c r="O56">
+        <v>5.397144273988666E-07</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57">
-        <v>91.91445839536388</v>
+        <v>91.91445839536385</v>
       </c>
       <c r="B57">
-        <v>428950.0467006704</v>
+        <v>428950.0467006684</v>
       </c>
       <c r="C57">
-        <v>634.3152047001389</v>
+        <v>634.3152047001357</v>
       </c>
       <c r="D57">
         <v>24951.33557515401</v>
       </c>
       <c r="E57">
-        <v>4861.303848727565</v>
+        <v>4861.303848727568</v>
       </c>
       <c r="F57">
         <v>4202.254160045183</v>
       </c>
       <c r="G57">
-        <v>6.690376625420791</v>
+        <v>6.690376625420835</v>
       </c>
       <c r="H57">
-        <v>28.13877835817159</v>
+        <v>28.13877835817167</v>
       </c>
       <c r="I57">
-        <v>6.225487556320068E-09</v>
+        <v>6.225487556320079E-09</v>
       </c>
       <c r="J57">
         <v>5.087645878435768E-09</v>
@@ -2840,59 +3182,71 @@
         <v>0.09625474130575878</v>
       </c>
       <c r="M57">
-        <v>691.874641745113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+        <v>0.09625418517377893</v>
+      </c>
+      <c r="N57">
+        <v>691.8746417451123</v>
+      </c>
+      <c r="O57">
+        <v>5.561319798589829E-07</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58">
-        <v>92.81594389566419</v>
+        <v>92.81594389566418</v>
       </c>
       <c r="B58">
-        <v>460808.9961560302</v>
+        <v>460808.99615603</v>
       </c>
       <c r="C58">
-        <v>679.3042460302571</v>
+        <v>679.304246030257</v>
       </c>
       <c r="D58">
         <v>24795.73353020646</v>
       </c>
       <c r="E58">
-        <v>4819.504651501669</v>
+        <v>4819.504651501668</v>
       </c>
       <c r="F58">
-        <v>4159.734497878643</v>
+        <v>4159.734497878642</v>
       </c>
       <c r="G58">
-        <v>6.638591315517391</v>
+        <v>6.63859131551737</v>
       </c>
       <c r="H58">
-        <v>28.54114245055111</v>
+        <v>28.5411424505511</v>
       </c>
       <c r="I58">
-        <v>6.4888256265761E-09</v>
+        <v>6.488825626576107E-09</v>
       </c>
       <c r="J58">
         <v>5.272265054157517E-09</v>
       </c>
       <c r="K58">
-        <v>9.774483880625337E-05</v>
+        <v>9.774483880625334E-05</v>
       </c>
       <c r="L58">
         <v>0.09472584868452771</v>
       </c>
       <c r="M58">
-        <v>682.8416836519009</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+        <v>0.09472527596326276</v>
+      </c>
+      <c r="N58">
+        <v>682.8416836519007</v>
+      </c>
+      <c r="O58">
+        <v>5.727212649567751E-07</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59">
         <v>93.7174293959645</v>
       </c>
       <c r="B59">
-        <v>494354.854712095</v>
+        <v>494354.8547120949</v>
       </c>
       <c r="C59">
-        <v>726.7313696519748</v>
+        <v>726.7313696519747</v>
       </c>
       <c r="D59">
         <v>24638.25787720591</v>
@@ -2922,18 +3276,24 @@
         <v>0.09322571696243424</v>
       </c>
       <c r="M59">
+        <v>0.09322512748239657</v>
+      </c>
+      <c r="N59">
         <v>673.7727345206213</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="O59">
+        <v>5.894800376655731E-07</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60">
-        <v>94.61891489626483</v>
+        <v>94.61891489626481</v>
       </c>
       <c r="B60">
-        <v>529638.7317084341</v>
+        <v>529638.7317084303</v>
       </c>
       <c r="C60">
-        <v>776.7050054176187</v>
+        <v>776.7050054176127</v>
       </c>
       <c r="D60">
         <v>24478.78541475914</v>
@@ -2945,10 +3305,10 @@
         <v>4072.422949335419</v>
       </c>
       <c r="G60">
-        <v>6.536702253082932</v>
+        <v>6.536702253082944</v>
       </c>
       <c r="H60">
-        <v>29.441021708565</v>
+        <v>29.44102170856497</v>
       </c>
       <c r="I60">
         <v>7.07183089917385E-09</v>
@@ -2957,162 +3317,186 @@
         <v>5.654585214948989E-09</v>
       </c>
       <c r="K60">
-        <v>9.267231330201798E-05</v>
+        <v>9.267231330201801E-05</v>
       </c>
       <c r="L60">
         <v>0.09175340308046945</v>
       </c>
       <c r="M60">
-        <v>664.6643460653702</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+        <v>0.09175279667300838</v>
+      </c>
+      <c r="N60">
+        <v>664.6643460653698</v>
+      </c>
+      <c r="O60">
+        <v>6.064074610656896E-07</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61">
         <v>95.52040039656514</v>
       </c>
       <c r="B61">
-        <v>566712.0223859546</v>
+        <v>566712.022385955</v>
       </c>
       <c r="C61">
-        <v>829.3402804623473</v>
+        <v>829.3402804623479</v>
       </c>
       <c r="D61">
-        <v>24317.18992925903</v>
+        <v>24317.18992925902</v>
       </c>
       <c r="E61">
-        <v>4687.582980144649</v>
+        <v>4687.58298014465</v>
       </c>
       <c r="F61">
         <v>4027.559268433585</v>
       </c>
       <c r="G61">
-        <v>6.486386422709768</v>
+        <v>6.486386422709774</v>
       </c>
       <c r="H61">
-        <v>29.94036282974114</v>
+        <v>29.94036282974116</v>
       </c>
       <c r="I61">
-        <v>7.395012745863472E-09</v>
+        <v>7.395012745863482E-09</v>
       </c>
       <c r="J61">
-        <v>5.852602667735166E-09</v>
+        <v>5.852602667735171E-09</v>
       </c>
       <c r="K61">
-        <v>9.024169503720646E-05</v>
+        <v>9.024169503720644E-05</v>
       </c>
       <c r="L61">
-        <v>0.09030702982723757</v>
+        <v>0.09030702982723755</v>
       </c>
       <c r="M61">
-        <v>655.5132622204236</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+        <v>0.09030640632312319</v>
+      </c>
+      <c r="N61">
+        <v>655.5132622204231</v>
+      </c>
+      <c r="O61">
+        <v>6.235041143641084E-07</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62">
         <v>96.42188589686545</v>
       </c>
       <c r="B62">
-        <v>605626.4277504031</v>
+        <v>605626.4277504014</v>
       </c>
       <c r="C62">
-        <v>884.7598205175627</v>
+        <v>884.7598205175602</v>
       </c>
       <c r="D62">
-        <v>24153.34180363353</v>
+        <v>24153.34180363352</v>
       </c>
       <c r="E62">
         <v>4641.275272602285</v>
       </c>
       <c r="F62">
-        <v>3981.840086108689</v>
+        <v>3981.840086108688</v>
       </c>
       <c r="G62">
-        <v>6.436389843083919</v>
+        <v>6.436389843083898</v>
       </c>
       <c r="H62">
-        <v>30.47416728907092</v>
+        <v>30.47416728907094</v>
       </c>
       <c r="I62">
-        <v>7.741998194673185E-09</v>
+        <v>7.741998194673194E-09</v>
       </c>
       <c r="J62">
-        <v>6.055443654710893E-09</v>
+        <v>6.055443654710897E-09</v>
       </c>
       <c r="K62">
-        <v>8.787652179683772E-05</v>
+        <v>8.787652179683768E-05</v>
       </c>
       <c r="L62">
-        <v>0.08888407639653145</v>
+        <v>0.0888840763965314</v>
       </c>
       <c r="M62">
-        <v>646.316420035361</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+        <v>0.08888343562454104</v>
+      </c>
+      <c r="N62">
+        <v>646.3164200353613</v>
+      </c>
+      <c r="O62">
+        <v>6.407719903539255E-07</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63">
-        <v>97.32337139716577</v>
+        <v>97.32337139716576</v>
       </c>
       <c r="B63">
-        <v>646433.9827391421</v>
+        <v>646433.9827391369</v>
       </c>
       <c r="C63">
-        <v>943.0946673645802</v>
+        <v>943.094667364571</v>
       </c>
       <c r="D63">
         <v>23987.10761618909</v>
       </c>
       <c r="E63">
-        <v>4593.715428065014</v>
+        <v>4593.715428065015</v>
       </c>
       <c r="F63">
         <v>3935.225529905423</v>
       </c>
       <c r="G63">
-        <v>6.386665129380224</v>
+        <v>6.386665129380209</v>
       </c>
       <c r="H63">
-        <v>31.04383174366809</v>
+        <v>31.04383174366812</v>
       </c>
       <c r="I63">
-        <v>8.115099224835028E-09</v>
+        <v>8.115099224835038E-09</v>
       </c>
       <c r="J63">
-        <v>6.263329936811015E-09</v>
+        <v>6.263329936811013E-09</v>
       </c>
       <c r="K63">
         <v>8.55734860920325E-05</v>
       </c>
       <c r="L63">
-        <v>0.08748162366421454</v>
+        <v>0.08748162366421451</v>
       </c>
       <c r="M63">
-        <v>637.0709480481686</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>0.08748096544973144</v>
+      </c>
+      <c r="N63">
+        <v>637.0709480481685</v>
+      </c>
+      <c r="O63">
+        <v>6.58214483075191E-07</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64">
         <v>98.22485689746608</v>
       </c>
       <c r="B64">
-        <v>689187.0936028546</v>
+        <v>689187.0936028538</v>
       </c>
       <c r="C64">
-        <v>1004.485330331235</v>
+        <v>1004.485330331234</v>
       </c>
       <c r="D64">
         <v>23818.34972717447</v>
       </c>
       <c r="E64">
-        <v>4544.848129429863</v>
+        <v>4544.848129429865</v>
       </c>
       <c r="F64">
-        <v>3887.673596327923</v>
+        <v>3887.673596327924</v>
       </c>
       <c r="G64">
-        <v>6.33718461601061</v>
+        <v>6.337184616010595</v>
       </c>
       <c r="H64">
-        <v>31.65097002596651</v>
+        <v>31.65097002596653</v>
       </c>
       <c r="I64">
         <v>8.516908149894616E-09</v>
@@ -3127,24 +3511,30 @@
         <v>0.08609655077671827</v>
       </c>
       <c r="M64">
-        <v>627.7741623255959</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+        <v>0.08609587494035191</v>
+      </c>
+      <c r="N64">
+        <v>627.7741623255962</v>
+      </c>
+      <c r="O64">
+        <v>6.758363663533981E-07</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65">
         <v>99.12634239776639</v>
       </c>
       <c r="B65">
-        <v>733938.5854949282</v>
+        <v>733938.5854949285</v>
       </c>
       <c r="C65">
-        <v>1069.082992493367</v>
+        <v>1069.082992493368</v>
       </c>
       <c r="D65">
         <v>23646.92585027125</v>
       </c>
       <c r="E65">
-        <v>4494.614695593056</v>
+        <v>4494.614695593055</v>
       </c>
       <c r="F65">
         <v>3839.139810068172</v>
@@ -3168,179 +3558,209 @@
         <v>0.08472568626475656</v>
       </c>
       <c r="M65">
+        <v>0.0847249926209928</v>
+      </c>
+      <c r="N65">
         <v>618.4235602803598</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="O65">
+        <v>6.936437637621861E-07</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66">
         <v>100.0278278980667</v>
       </c>
       <c r="B66">
-        <v>780741.7613365301</v>
+        <v>780741.7613365294</v>
       </c>
       <c r="C66">
-        <v>1137.050895396265</v>
+        <v>1137.050895396264</v>
       </c>
       <c r="D66">
         <v>23472.68860563382</v>
       </c>
       <c r="E66">
-        <v>4442.952621754255</v>
+        <v>4442.952621754262</v>
       </c>
       <c r="F66">
-        <v>3789.576851851748</v>
+        <v>3789.576851851753</v>
       </c>
       <c r="G66">
-        <v>6.238935460411226</v>
+        <v>6.238935460411232</v>
       </c>
       <c r="H66">
-        <v>32.98532549856353</v>
+        <v>32.98532549856358</v>
       </c>
       <c r="I66">
-        <v>9.418675440511231E-09</v>
+        <v>9.418675440511246E-09</v>
       </c>
       <c r="J66">
-        <v>6.919907096647077E-09</v>
+        <v>6.919907096647082E-09</v>
       </c>
       <c r="K66">
         <v>7.900818097347758E-05</v>
       </c>
       <c r="L66">
-        <v>0.08336592041194803</v>
+        <v>0.08336592041194801</v>
       </c>
       <c r="M66">
-        <v>609.0168123002911</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
+        <v>0.08336520876783754</v>
+      </c>
+      <c r="N66">
+        <v>609.0168123002909</v>
+      </c>
+      <c r="O66">
+        <v>7.116441104755229E-07</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67">
         <v>100.929313398367</v>
       </c>
       <c r="B67">
-        <v>829650.4730935657</v>
+        <v>829650.4730935746</v>
       </c>
       <c r="C67">
-        <v>1208.565929702798</v>
+        <v>1208.565929702816</v>
       </c>
       <c r="D67">
-        <v>23295.48505030201</v>
+        <v>23295.48505030203</v>
       </c>
       <c r="E67">
-        <v>4389.795079039773</v>
+        <v>4389.795079039766</v>
       </c>
       <c r="F67">
-        <v>3738.934150573086</v>
+        <v>3738.934150573087</v>
       </c>
       <c r="G67">
-        <v>6.190198170426647</v>
+        <v>6.190198170426631</v>
       </c>
       <c r="H67">
-        <v>33.71704671034136</v>
+        <v>33.71704671034109</v>
       </c>
       <c r="I67">
-        <v>9.925629454954611E-09</v>
+        <v>9.925629454954503E-09</v>
       </c>
       <c r="J67">
-        <v>7.150775405243463E-09</v>
+        <v>7.150775405243445E-09</v>
       </c>
       <c r="K67">
-        <v>7.692574262280448E-05</v>
+        <v>7.692574262280471E-05</v>
       </c>
       <c r="L67">
-        <v>0.08201428683569195</v>
+        <v>0.08201428683569209</v>
       </c>
       <c r="M67">
-        <v>599.5517511552806</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13">
+        <v>0.08201355698958476</v>
+      </c>
+      <c r="N67">
+        <v>599.5517511552825</v>
+      </c>
+      <c r="O67">
+        <v>7.298461073341514E-07</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68">
-        <v>101.8307988986674</v>
+        <v>101.8307988986673</v>
       </c>
       <c r="B68">
-        <v>880719.2066529994</v>
+        <v>880719.2066530107</v>
       </c>
       <c r="C68">
-        <v>1283.820463225482</v>
+        <v>1283.820463225504</v>
       </c>
       <c r="D68">
-        <v>23115.15618072753</v>
+        <v>23115.15618072754</v>
       </c>
       <c r="E68">
-        <v>4335.070369152387</v>
+        <v>4335.070369152378</v>
       </c>
       <c r="F68">
-        <v>3687.157434994668</v>
+        <v>3687.15743499466</v>
       </c>
       <c r="G68">
-        <v>6.141766259523898</v>
+        <v>6.141766259523894</v>
       </c>
       <c r="H68">
-        <v>34.49531255201268</v>
+        <v>34.49531255201269</v>
       </c>
       <c r="I68">
-        <v>1.047540826679515E-08</v>
+        <v>1.047540826679514E-08</v>
       </c>
       <c r="J68">
-        <v>7.388250012315317E-09</v>
+        <v>7.388250012315314E-09</v>
       </c>
       <c r="K68">
-        <v>7.489241534903618E-05</v>
+        <v>7.489241534903624E-05</v>
       </c>
       <c r="L68">
-        <v>0.08066802100246853</v>
+        <v>0.08066802100246857</v>
       </c>
       <c r="M68">
-        <v>590.026359083725</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+        <v>0.08066727274280124</v>
+      </c>
+      <c r="N68">
+        <v>590.0263590837252</v>
+      </c>
+      <c r="O68">
+        <v>7.482596673409998E-07</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69">
-        <v>102.7322843989677</v>
+        <v>102.7322843989676</v>
       </c>
       <c r="B69">
-        <v>934003.1815095396</v>
+        <v>934003.1815095289</v>
       </c>
       <c r="C69">
-        <v>1363.024442305538</v>
+        <v>1363.024442305518</v>
       </c>
       <c r="D69">
         <v>22931.53640069948</v>
       </c>
       <c r="E69">
-        <v>4278.701329605939</v>
+        <v>4278.701329605943</v>
       </c>
       <c r="F69">
-        <v>3634.188239869935</v>
+        <v>3634.188239869938</v>
       </c>
       <c r="G69">
-        <v>6.093694116552514</v>
+        <v>6.093694116552516</v>
       </c>
       <c r="H69">
-        <v>35.32320396475996</v>
+        <v>35.32320396475999</v>
       </c>
       <c r="I69">
         <v>1.107279640947901E-08</v>
       </c>
       <c r="J69">
-        <v>7.632746217679932E-09</v>
+        <v>7.632746217679928E-09</v>
       </c>
       <c r="K69">
-        <v>7.29060545466019E-05</v>
+        <v>7.290605454660188E-05</v>
       </c>
       <c r="L69">
         <v>0.07932460236835671</v>
       </c>
       <c r="M69">
-        <v>580.438752401857</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
+        <v>0.07932383547250195</v>
+      </c>
+      <c r="N69">
+        <v>580.4387524018571</v>
+      </c>
+      <c r="O69">
+        <v>7.668958547661249E-07</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70">
         <v>103.633769899268</v>
       </c>
       <c r="B70">
-        <v>989558.4664554443</v>
+        <v>989558.4664554438</v>
       </c>
       <c r="C70">
         <v>1446.407807410995</v>
@@ -3349,16 +3769,16 @@
         <v>22744.45294601448</v>
       </c>
       <c r="E70">
-        <v>4220.604685070876</v>
+        <v>4220.604685070878</v>
       </c>
       <c r="F70">
-        <v>3579.963360950327</v>
+        <v>3579.963360950329</v>
       </c>
       <c r="G70">
-        <v>6.046051064507324</v>
+        <v>6.046051064507322</v>
       </c>
       <c r="H70">
-        <v>36.20421739852967</v>
+        <v>36.20421739852968</v>
       </c>
       <c r="I70">
         <v>1.172325336860507E-08</v>
@@ -3373,71 +3793,83 @@
         <v>0.07798178547291396</v>
       </c>
       <c r="M70">
+        <v>0.07798099970609705</v>
+      </c>
+      <c r="N70">
         <v>570.7871634277825</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="O70">
+        <v>7.857668169036615E-07</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71">
         <v>104.5352553995683</v>
       </c>
       <c r="B71">
-        <v>1047442.112379235</v>
+        <v>1047442.112379225</v>
       </c>
       <c r="C71">
-        <v>1534.223268984495</v>
+        <v>1534.223268984476</v>
       </c>
       <c r="D71">
-        <v>22553.72525466019</v>
+        <v>22553.7252546602</v>
       </c>
       <c r="E71">
-        <v>4160.690340553237</v>
+        <v>4160.690340553243</v>
       </c>
       <c r="F71">
-        <v>3524.414253020283</v>
+        <v>3524.414253020285</v>
       </c>
       <c r="G71">
-        <v>5.998921372749636</v>
+        <v>5.998921372749638</v>
       </c>
       <c r="H71">
-        <v>37.14232830399088</v>
+        <v>37.14232830399084</v>
       </c>
       <c r="I71">
-        <v>1.243303165652325E-08</v>
+        <v>1.243303165652323E-08</v>
       </c>
       <c r="J71">
-        <v>8.144664404742799E-09</v>
+        <v>8.144664404742791E-09</v>
       </c>
       <c r="K71">
-        <v>6.90660928533238E-05</v>
+        <v>6.906609285332391E-05</v>
       </c>
       <c r="L71">
-        <v>0.07663762390663323</v>
+        <v>0.07663762390663327</v>
       </c>
       <c r="M71">
-        <v>561.0699194684248</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
+        <v>0.07663681902092472</v>
+      </c>
+      <c r="N71">
+        <v>561.069919468425</v>
+      </c>
+      <c r="O71">
+        <v>8.048857085550588E-07</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72">
         <v>105.4367408998686</v>
       </c>
       <c r="B72">
-        <v>1107712.303090649</v>
+        <v>1107712.303090637</v>
       </c>
       <c r="C72">
-        <v>1626.749494682458</v>
+        <v>1626.749494682434</v>
       </c>
       <c r="D72">
         <v>22359.16426787741</v>
       </c>
       <c r="E72">
-        <v>4098.860612716592</v>
+        <v>4098.860612716597</v>
       </c>
       <c r="F72">
-        <v>3467.466364977502</v>
+        <v>3467.466364977504</v>
       </c>
       <c r="G72">
-        <v>5.952404451932711</v>
+        <v>5.95240445193271</v>
       </c>
       <c r="H72">
         <v>38.14206940448418</v>
@@ -3455,174 +3887,204 @@
         <v>0.07529048977234734</v>
       </c>
       <c r="M72">
+        <v>0.07528966550573804</v>
+      </c>
+      <c r="N72">
         <v>551.2854185840902</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="O72">
+        <v>8.242666092950279E-07</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73">
         <v>106.3382264001689</v>
       </c>
       <c r="B73">
-        <v>1170428.52474832</v>
+        <v>1170428.524748325</v>
       </c>
       <c r="C73">
-        <v>1724.294763661419</v>
+        <v>1724.294763661429</v>
       </c>
       <c r="D73">
-        <v>22160.57164298163</v>
+        <v>22160.57164298164</v>
       </c>
       <c r="E73">
-        <v>4035.009396887373</v>
+        <v>4035.009396887376</v>
       </c>
       <c r="F73">
-        <v>3409.038406214336</v>
+        <v>3409.038406214342</v>
       </c>
       <c r="G73">
-        <v>5.906615219937345</v>
+        <v>5.906615219937336</v>
       </c>
       <c r="H73">
-        <v>39.20862762650045</v>
+        <v>39.2086276265003</v>
       </c>
       <c r="I73">
-        <v>1.40604204014625E-08</v>
+        <v>1.406042040146242E-08</v>
       </c>
       <c r="J73">
-        <v>8.690691185584666E-09</v>
+        <v>8.690691185584648E-09</v>
       </c>
       <c r="K73">
-        <v>6.539021309598076E-05</v>
+        <v>6.539021309598091E-05</v>
       </c>
       <c r="L73">
-        <v>0.0739390901362475</v>
+        <v>0.07393909013624758</v>
       </c>
       <c r="M73">
-        <v>541.4321018237652</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
+        <v>0.07393824621181394</v>
+      </c>
+      <c r="N73">
+        <v>541.4321018237659</v>
+      </c>
+      <c r="O73">
+        <v>8.4392443364237E-07</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74">
         <v>107.2397119004692</v>
       </c>
       <c r="B74">
-        <v>1235651.753898016</v>
+        <v>1235651.753898015</v>
       </c>
       <c r="C74">
-        <v>1827.201146537169</v>
+        <v>1827.201146537167</v>
       </c>
       <c r="D74">
-        <v>21957.73885292615</v>
+        <v>21957.73885292616</v>
       </c>
       <c r="E74">
-        <v>3969.021269535477</v>
+        <v>3969.021269535478</v>
       </c>
       <c r="F74">
         <v>3349.041539434745</v>
       </c>
       <c r="G74">
-        <v>5.861684629635922</v>
+        <v>5.861684629635914</v>
       </c>
       <c r="H74">
-        <v>40.34796474644151</v>
+        <v>40.34796474644146</v>
       </c>
       <c r="I74">
-        <v>1.49959613990582E-08</v>
+        <v>1.499596139905816E-08</v>
       </c>
       <c r="J74">
-        <v>8.97800545390851E-09</v>
+        <v>8.978005453908511E-09</v>
       </c>
       <c r="K74">
-        <v>6.360912490672753E-05</v>
+        <v>6.360912490672759E-05</v>
       </c>
       <c r="L74">
-        <v>0.07258248103249812</v>
+        <v>0.07258248103249819</v>
       </c>
       <c r="M74">
-        <v>531.5084216164489</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
+        <v>0.07258161715766376</v>
+      </c>
+      <c r="N74">
+        <v>531.5084216164494</v>
+      </c>
+      <c r="O74">
+        <v>8.638748344364758E-07</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75">
-        <v>108.1411974007696</v>
+        <v>108.1411974007695</v>
       </c>
       <c r="B75">
-        <v>1303444.663228126</v>
+        <v>1303444.663228137</v>
       </c>
       <c r="C75">
-        <v>1935.849269514974</v>
+        <v>1935.849269515</v>
       </c>
       <c r="D75">
         <v>21750.44613983211</v>
       </c>
       <c r="E75">
-        <v>3900.770529844139</v>
+        <v>3900.770529844134</v>
       </c>
       <c r="F75">
-        <v>3287.378496978506</v>
+        <v>3287.378496978503</v>
       </c>
       <c r="G75">
-        <v>5.817760351794511</v>
+        <v>5.81776035179453</v>
       </c>
       <c r="H75">
-        <v>41.56696838531515</v>
+        <v>41.56696838531522</v>
       </c>
       <c r="I75">
-        <v>1.602716962087761E-08</v>
+        <v>1.602716962087762E-08</v>
       </c>
       <c r="J75">
-        <v>9.275767533847998E-09</v>
+        <v>9.275767533847993E-09</v>
       </c>
       <c r="K75">
-        <v>6.186350863702565E-05</v>
+        <v>6.186350863702567E-05</v>
       </c>
       <c r="L75">
-        <v>0.07122007884097056</v>
+        <v>0.07122007884097059</v>
       </c>
       <c r="M75">
-        <v>521.5128060112069</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
+        <v>0.07121919470687069</v>
+      </c>
+      <c r="N75">
+        <v>521.5128060112066</v>
+      </c>
+      <c r="O75">
+        <v>8.841340999070958E-07</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76">
         <v>109.0426829010699</v>
       </c>
       <c r="B76">
-        <v>1373871.84276401</v>
+        <v>1373871.84276402</v>
       </c>
       <c r="C76">
-        <v>2050.663715477082</v>
+        <v>2050.663715477102</v>
       </c>
       <c r="D76">
         <v>21538.4612794928</v>
       </c>
       <c r="E76">
-        <v>3830.120190165244</v>
+        <v>3830.12019016524</v>
       </c>
       <c r="F76">
-        <v>3223.942621346006</v>
+        <v>3223.942621346003</v>
       </c>
       <c r="G76">
         <v>5.775007609152518</v>
       </c>
       <c r="H76">
-        <v>42.87364210288484</v>
+        <v>42.87364210288477</v>
       </c>
       <c r="I76">
-        <v>1.716720433068634E-08</v>
+        <v>1.716720433068631E-08</v>
       </c>
       <c r="J76">
-        <v>9.584739164910582E-09</v>
+        <v>9.584739164910581E-09</v>
       </c>
       <c r="K76">
-        <v>6.01515751389987E-05</v>
+        <v>6.015157513899871E-05</v>
       </c>
       <c r="L76">
-        <v>0.06985166828669223</v>
+        <v>0.06985166828669227</v>
       </c>
       <c r="M76">
-        <v>511.4436184798853</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
+        <v>0.06985076356764691</v>
+      </c>
+      <c r="N76">
+        <v>511.4436184798855</v>
+      </c>
+      <c r="O76">
+        <v>9.047190453597843E-07</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77">
         <v>109.9441684013702</v>
       </c>
@@ -3636,92 +4098,104 @@
         <v>21321.53810034557</v>
       </c>
       <c r="E77">
-        <v>3756.92093479643</v>
+        <v>3756.920934796422</v>
       </c>
       <c r="F77">
-        <v>3158.616836830552</v>
+        <v>3158.616836830546</v>
       </c>
       <c r="G77">
-        <v>5.73361016093827</v>
+        <v>5.733610160938255</v>
       </c>
       <c r="H77">
-        <v>44.27734622759201</v>
+        <v>44.2773462275918</v>
       </c>
       <c r="I77">
-        <v>1.843158194493797E-08</v>
+        <v>1.843158194493786E-08</v>
       </c>
       <c r="J77">
-        <v>9.905750329409255E-09</v>
+        <v>9.905750329409246E-09</v>
       </c>
       <c r="K77">
-        <v>5.847155953604046E-05</v>
+        <v>5.847155953604051E-05</v>
       </c>
       <c r="L77">
-        <v>0.06847740589870577</v>
+        <v>0.06847740589870581</v>
       </c>
       <c r="M77">
-        <v>501.2991130271644</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13">
+        <v>0.06847648025180499</v>
+      </c>
+      <c r="N77">
+        <v>501.2991130271652</v>
+      </c>
+      <c r="O77">
+        <v>9.256469008246532E-07</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78">
         <v>110.8456539016705</v>
       </c>
       <c r="B78">
-        <v>1522898.356484858</v>
+        <v>1522898.356484868</v>
       </c>
       <c r="C78">
-        <v>2300.746826930051</v>
+        <v>2300.746826930077</v>
       </c>
       <c r="D78">
-        <v>21099.41468241729</v>
+        <v>21099.41468241732</v>
       </c>
       <c r="E78">
-        <v>3681.010081087792</v>
+        <v>3681.010081087776</v>
       </c>
       <c r="F78">
-        <v>3091.272569250558</v>
+        <v>3091.272569250547</v>
       </c>
       <c r="G78">
-        <v>5.693771441276608</v>
+        <v>5.693771441276621</v>
       </c>
       <c r="H78">
-        <v>45.78910503063322</v>
+        <v>45.78910503063282</v>
       </c>
       <c r="I78">
-        <v>1.98387164425132E-08</v>
+        <v>1.983871644251287E-08</v>
       </c>
       <c r="J78">
-        <v>1.023970654011909E-08</v>
+        <v>1.023970654011905E-08</v>
       </c>
       <c r="K78">
-        <v>5.682172203142552E-05</v>
+        <v>5.682172203142577E-05</v>
       </c>
       <c r="L78">
-        <v>0.0670978175047251</v>
+        <v>0.06709781750472534</v>
       </c>
       <c r="M78">
-        <v>491.077384380622</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
+        <v>0.0670968705695285</v>
+      </c>
+      <c r="N78">
+        <v>491.0773843806242</v>
+      </c>
+      <c r="O78">
+        <v>9.469351968374533E-07</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79">
         <v>111.7471394019708</v>
       </c>
       <c r="B79">
-        <v>1601638.554053101</v>
+        <v>1601638.554053094</v>
       </c>
       <c r="C79">
-        <v>2437.142483793295</v>
+        <v>2437.142483793277</v>
       </c>
       <c r="D79">
         <v>20871.81113758325</v>
       </c>
       <c r="E79">
-        <v>3602.210598254981</v>
+        <v>3602.210598254983</v>
       </c>
       <c r="F79">
-        <v>3021.768646453331</v>
+        <v>3021.768646453332</v>
       </c>
       <c r="G79">
         <v>5.655715860758164</v>
@@ -3742,33 +4216,39 @@
         <v>0.06571378821815936</v>
       </c>
       <c r="M79">
+        <v>0.06571281961650795</v>
+      </c>
+      <c r="N79">
         <v>480.7763130354255</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="O79">
+        <v>9.686016514117468E-07</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80">
-        <v>112.6486249022712</v>
+        <v>112.6486249022711</v>
       </c>
       <c r="B80">
-        <v>1683295.177150825</v>
+        <v>1683295.177150838</v>
       </c>
       <c r="C80">
-        <v>2581.973726943895</v>
+        <v>2581.973726943932</v>
       </c>
       <c r="D80">
-        <v>20638.42683961276</v>
+        <v>20638.42683961277</v>
       </c>
       <c r="E80">
-        <v>3520.330269566401</v>
+        <v>3520.330269566385</v>
       </c>
       <c r="F80">
-        <v>2949.95023569486</v>
+        <v>2949.950235694848</v>
       </c>
       <c r="G80">
-        <v>5.619690288908053</v>
+        <v>5.619690288908084</v>
       </c>
       <c r="H80">
-        <v>49.19168797401299</v>
+        <v>49.19168797401301</v>
       </c>
       <c r="I80">
         <v>2.317377951056382E-08</v>
@@ -3777,121 +4257,139 @@
         <v>1.095050810030644E-08</v>
       </c>
       <c r="K80">
-        <v>5.360576286235097E-05</v>
+        <v>5.360576286235102E-05</v>
       </c>
       <c r="L80">
-        <v>0.0643265433868949</v>
+        <v>0.06432654338689495</v>
       </c>
       <c r="M80">
-        <v>470.3935048608943</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13">
+        <v>0.06432555272283232</v>
+      </c>
+      <c r="N80">
+        <v>470.3935048608942</v>
+      </c>
+      <c r="O80">
+        <v>9.906640626339897E-07</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81">
-        <v>113.5501104025715</v>
+        <v>113.5501104025714</v>
       </c>
       <c r="B81">
-        <v>1767945.739071117</v>
+        <v>1767945.739071077</v>
       </c>
       <c r="C81">
-        <v>2735.98838930898</v>
+        <v>2735.988389308875</v>
       </c>
       <c r="D81">
-        <v>20398.93692710314</v>
+        <v>20398.93692710313</v>
       </c>
       <c r="E81">
-        <v>3435.161124721325</v>
+        <v>3435.161124721359</v>
       </c>
       <c r="F81">
-        <v>2875.647907574985</v>
+        <v>2875.647907575007</v>
       </c>
       <c r="G81">
-        <v>5.585965747968418</v>
+        <v>5.585965747968444</v>
       </c>
       <c r="H81">
-        <v>51.11705514520717</v>
+        <v>51.11705514520735</v>
       </c>
       <c r="I81">
-        <v>2.516039914641358E-08</v>
+        <v>2.516039914641374E-08</v>
       </c>
       <c r="J81">
-        <v>1.132963062428621E-08</v>
+        <v>1.132963062428622E-08</v>
       </c>
       <c r="K81">
-        <v>5.203631284130686E-05</v>
+        <v>5.203631284130683E-05</v>
       </c>
       <c r="L81">
-        <v>0.06293761910460428</v>
+        <v>0.06293761910460424</v>
       </c>
       <c r="M81">
-        <v>459.9262247664776</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13">
+        <v>0.06293660596439113</v>
+      </c>
+      <c r="N81">
+        <v>459.9262247664764</v>
+      </c>
+      <c r="O81">
+        <v>1.013140213114953E-06</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82">
         <v>114.4515959028718</v>
       </c>
       <c r="B82">
-        <v>1855670.76715769</v>
+        <v>1855670.767157694</v>
       </c>
       <c r="C82">
-        <v>2900.022311011199</v>
+        <v>2900.022311011209</v>
       </c>
       <c r="D82">
-        <v>20152.98783868665</v>
+        <v>20152.98783868667</v>
       </c>
       <c r="E82">
-        <v>3346.479321793637</v>
+        <v>3346.479321793639</v>
       </c>
       <c r="F82">
-        <v>2798.676961813432</v>
+        <v>2798.676961813438</v>
       </c>
       <c r="G82">
-        <v>5.554839367728744</v>
+        <v>5.554839367728739</v>
       </c>
       <c r="H82">
-        <v>53.22111259736643</v>
+        <v>53.22111259736603</v>
       </c>
       <c r="I82">
-        <v>2.74099272212428E-08</v>
+        <v>2.740992722124251E-08</v>
       </c>
       <c r="J82">
-        <v>1.172628169739477E-08</v>
+        <v>1.172628169739476E-08</v>
       </c>
       <c r="K82">
-        <v>5.049039098564287E-05</v>
+        <v>5.049039098564294E-05</v>
       </c>
       <c r="L82">
-        <v>0.06154882111075571</v>
+        <v>0.06154882111075578</v>
       </c>
       <c r="M82">
-        <v>449.3713234529466</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13">
+        <v>0.06154778506296083</v>
+      </c>
+      <c r="N82">
+        <v>449.3713234529478</v>
+      </c>
+      <c r="O82">
+        <v>1.036047794948706E-06</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83">
         <v>115.3530814031721</v>
       </c>
       <c r="B83">
-        <v>1946553.705599691</v>
+        <v>1946553.705599681</v>
       </c>
       <c r="C83">
-        <v>3075.006103353453</v>
+        <v>3075.006103353428</v>
       </c>
       <c r="D83">
-        <v>19900.19154876664</v>
+        <v>19900.19154876665</v>
       </c>
       <c r="E83">
-        <v>3254.045718729789</v>
+        <v>3254.045718729795</v>
       </c>
       <c r="F83">
-        <v>2718.837207451358</v>
+        <v>2718.837207451361</v>
       </c>
       <c r="G83">
-        <v>5.526636680903099</v>
+        <v>5.526636680903089</v>
       </c>
       <c r="H83">
-        <v>55.53216618228531</v>
+        <v>55.5321661822854</v>
       </c>
       <c r="I83">
         <v>2.997121614988973E-08</v>
@@ -3900,247 +4398,283 @@
         <v>1.214192220804689E-08</v>
       </c>
       <c r="K83">
-        <v>4.896642695622877E-05</v>
+        <v>4.896642695622879E-05</v>
       </c>
       <c r="L83">
-        <v>0.06016217118476624</v>
+        <v>0.06016217118476627</v>
       </c>
       <c r="M83">
-        <v>438.7251553530518</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+        <v>0.06016111178039894</v>
+      </c>
+      <c r="N83">
+        <v>438.7251553530521</v>
+      </c>
+      <c r="O83">
+        <v>1.05940436732979E-06</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84">
         <v>116.2545669034724</v>
       </c>
       <c r="B84">
-        <v>2040680.590321429</v>
+        <v>2040680.590321433</v>
       </c>
       <c r="C84">
-        <v>3261.969663311581</v>
+        <v>3261.969663311595</v>
       </c>
       <c r="D84">
-        <v>19640.11803929347</v>
+        <v>19640.11803929346</v>
       </c>
       <c r="E84">
-        <v>3157.60743085478</v>
+        <v>3157.607430854778</v>
       </c>
       <c r="F84">
-        <v>2635.913452819067</v>
+        <v>2635.913452819065</v>
       </c>
       <c r="G84">
         <v>5.501714384768819</v>
       </c>
       <c r="H84">
-        <v>58.08540945310275</v>
+        <v>58.08540945310308</v>
       </c>
       <c r="I84">
-        <v>3.290543604962021E-08</v>
+        <v>3.290543604962044E-08</v>
       </c>
       <c r="J84">
-        <v>1.257818330707829E-08</v>
+        <v>1.25781833070783E-08</v>
       </c>
       <c r="K84">
-        <v>4.74628871862239E-05</v>
+        <v>4.746288718622387E-05</v>
       </c>
       <c r="L84">
-        <v>0.05877984041227708</v>
+        <v>0.05877984041227705</v>
       </c>
       <c r="M84">
-        <v>427.9834842084598</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+        <v>0.05877875718491329</v>
+      </c>
+      <c r="N84">
+        <v>427.9834842084592</v>
+      </c>
+      <c r="O84">
+        <v>1.083227363756629E-06</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85">
         <v>117.1560524037727</v>
       </c>
       <c r="B85">
-        <v>2138139.393016455</v>
+        <v>2138139.39301646</v>
       </c>
       <c r="C85">
-        <v>3462.042811025548</v>
+        <v>3462.042811025562</v>
       </c>
       <c r="D85">
-        <v>19372.28534639979</v>
+        <v>19372.2853463998</v>
       </c>
       <c r="E85">
-        <v>3056.900693370153</v>
+        <v>3056.900693370145</v>
       </c>
       <c r="F85">
-        <v>2549.677009767821</v>
+        <v>2549.677009767814</v>
       </c>
       <c r="G85">
-        <v>5.480463766936885</v>
+        <v>5.480463766936877</v>
       </c>
       <c r="H85">
-        <v>60.92510844736189</v>
+        <v>60.92510844736183</v>
       </c>
       <c r="I85">
-        <v>3.629013547320498E-08</v>
+        <v>3.629013547320488E-08</v>
       </c>
       <c r="J85">
-        <v>1.30368999566468E-08</v>
+        <v>1.303689995664678E-08</v>
       </c>
       <c r="K85">
-        <v>4.597826726835372E-05</v>
+        <v>4.597826726835376E-05</v>
       </c>
       <c r="L85">
-        <v>0.05740406888254655</v>
+        <v>0.05740406888254659</v>
       </c>
       <c r="M85">
-        <v>417.141369919672</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
+        <v>0.05740296134837381</v>
+      </c>
+      <c r="N85">
+        <v>417.1413699196724</v>
+      </c>
+      <c r="O85">
+        <v>1.107534172772855E-06</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86">
-        <v>118.0575379040731</v>
+        <v>118.057537904073</v>
       </c>
       <c r="B86">
-        <v>2239018.904554072</v>
+        <v>2239018.90455407</v>
       </c>
       <c r="C86">
-        <v>3676.450047402911</v>
+        <v>3676.450047402907</v>
       </c>
       <c r="D86">
-        <v>19096.14622484109</v>
+        <v>19096.14622484112</v>
       </c>
       <c r="E86">
-        <v>2951.655275612093</v>
+        <v>2951.655275612096</v>
       </c>
       <c r="F86">
-        <v>2459.88850888177</v>
+        <v>2459.888508881774</v>
       </c>
       <c r="G86">
-        <v>5.463315106091678</v>
+        <v>5.463315106091668</v>
       </c>
       <c r="H86">
-        <v>64.10765304603679</v>
+        <v>64.10765304603655</v>
       </c>
       <c r="I86">
-        <v>4.022499405757054E-08</v>
+        <v>4.022499405757011E-08</v>
       </c>
       <c r="J86">
-        <v>1.352015504475261E-08</v>
+        <v>1.352015504475258E-08</v>
       </c>
       <c r="K86">
-        <v>4.451107606599958E-05</v>
+        <v>4.451107606599973E-05</v>
       </c>
       <c r="L86">
-        <v>0.05603707135294986</v>
+        <v>0.05603707135295</v>
       </c>
       <c r="M86">
-        <v>406.1930257596378</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
+        <v>0.05603593901062362</v>
+      </c>
+      <c r="N86">
+        <v>406.1930257596392</v>
+      </c>
+      <c r="O86">
+        <v>1.132342326373789E-06</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87">
         <v>118.9590234043734</v>
       </c>
       <c r="B87">
-        <v>2343407.006204688</v>
+        <v>2343407.006204678</v>
       </c>
       <c r="C87">
-        <v>3906.497414101144</v>
+        <v>3906.497414101112</v>
       </c>
       <c r="D87">
-        <v>18811.07002237645</v>
+        <v>18811.07002237641</v>
       </c>
       <c r="E87">
-        <v>2841.600418059001</v>
+        <v>2841.600418059004</v>
       </c>
       <c r="F87">
-        <v>2366.302173968062</v>
+        <v>2366.30217396806</v>
       </c>
       <c r="G87">
-        <v>5.450743535596019</v>
+        <v>5.450743535596035</v>
       </c>
       <c r="H87">
-        <v>67.70590437466099</v>
+        <v>67.70590437466193</v>
       </c>
       <c r="I87">
-        <v>4.48401408598741E-08</v>
+        <v>4.484014085987517E-08</v>
       </c>
       <c r="J87">
-        <v>1.403033839103305E-08</v>
+        <v>1.403033839103311E-08</v>
       </c>
       <c r="K87">
-        <v>4.305980775065186E-05</v>
+        <v>4.305980775065161E-05</v>
       </c>
       <c r="L87">
-        <v>0.05468092804505433</v>
+        <v>0.05468092804505412</v>
       </c>
       <c r="M87">
-        <v>395.1316279912253</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
+        <v>0.05467977037520896</v>
+      </c>
+      <c r="N87">
+        <v>395.1316279912228</v>
+      </c>
+      <c r="O87">
+        <v>1.157669845157894E-06</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88">
         <v>119.8605089046737</v>
       </c>
       <c r="B88">
-        <v>2451388.173002977</v>
+        <v>2451388.173002931</v>
       </c>
       <c r="C88">
-        <v>4153.55033972602</v>
+        <v>4153.55033972585</v>
       </c>
       <c r="D88">
-        <v>18516.31766085299</v>
+        <v>18516.31766085296</v>
       </c>
       <c r="E88">
-        <v>2726.471614815187</v>
+        <v>2726.471614815236</v>
       </c>
       <c r="F88">
-        <v>2268.671275526093</v>
+        <v>2268.671275526127</v>
       </c>
       <c r="G88">
-        <v>5.443277135111273</v>
+        <v>5.443277135111252</v>
       </c>
       <c r="H88">
-        <v>71.81553273172185</v>
+        <v>71.81553273172226</v>
       </c>
       <c r="I88">
-        <v>5.030846607148059E-08</v>
+        <v>5.030846607148112E-08</v>
       </c>
       <c r="J88">
-        <v>1.457022714019019E-08</v>
+        <v>1.457022714019022E-08</v>
       </c>
       <c r="K88">
-        <v>4.162289654552044E-05</v>
+        <v>4.162289654552033E-05</v>
       </c>
       <c r="L88">
-        <v>0.05333745882713403</v>
+        <v>0.05333745882713392</v>
       </c>
       <c r="M88">
-        <v>383.9490493943118</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13">
+        <v>0.05333627529132245</v>
+      </c>
+      <c r="N88">
+        <v>383.949049394311</v>
+      </c>
+      <c r="O88">
+        <v>1.183535811476245E-06</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89">
         <v>120.761994404974</v>
       </c>
       <c r="B89">
-        <v>2563040.088017601</v>
+        <v>2563040.088017623</v>
       </c>
       <c r="C89">
-        <v>4419.004061262101</v>
+        <v>4419.004061262197</v>
       </c>
       <c r="D89">
-        <v>18211.00653481222</v>
+        <v>18211.00653481223</v>
       </c>
       <c r="E89">
-        <v>2606.016327573083</v>
+        <v>2606.016327573061</v>
       </c>
       <c r="F89">
-        <v>2166.753579321265</v>
+        <v>2166.75357932125</v>
       </c>
       <c r="G89">
-        <v>5.441508448691224</v>
+        <v>5.441508448691232</v>
       </c>
       <c r="H89">
-        <v>76.56450548644693</v>
+        <v>76.56450548644686</v>
       </c>
       <c r="I89">
-        <v>5.686433491014065E-08</v>
+        <v>5.686433491014054E-08</v>
       </c>
       <c r="J89">
         <v>1.514309749493462E-08</v>
@@ -4149,502 +4683,580 @@
         <v>4.019864689974631E-05</v>
       </c>
       <c r="L89">
-        <v>0.05200807733040042</v>
+        <v>0.05200807733040044</v>
       </c>
       <c r="M89">
+        <v>0.05200686736912587</v>
+      </c>
+      <c r="N89">
         <v>372.63547305943</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="O89">
+        <v>1.209961274562603E-06</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90">
         <v>121.6634799052743</v>
       </c>
       <c r="B90">
-        <v>2678429.345212947</v>
+        <v>2678429.345212977</v>
       </c>
       <c r="C90">
-        <v>4704.253828043475</v>
+        <v>4704.253828043623</v>
       </c>
       <c r="D90">
-        <v>17894.06040591454</v>
+        <v>17894.06040591461</v>
       </c>
       <c r="E90">
-        <v>2479.994703267164</v>
+        <v>2479.994703267129</v>
       </c>
       <c r="F90">
-        <v>2060.314024804544</v>
+        <v>2060.314024804524</v>
       </c>
       <c r="G90">
-        <v>5.44611130828345</v>
+        <v>5.446111308283415</v>
       </c>
       <c r="H90">
-        <v>82.12773126209309</v>
+        <v>82.12773126209029</v>
       </c>
       <c r="I90">
-        <v>6.48329183924197E-08</v>
+        <v>6.483291839241658E-08</v>
       </c>
       <c r="J90">
-        <v>1.575288337364174E-08</v>
+        <v>1.575288337364164E-08</v>
       </c>
       <c r="K90">
-        <v>3.878512873702624E-05</v>
+        <v>3.878512873702653E-05</v>
       </c>
       <c r="L90">
-        <v>0.05069361860261656</v>
+        <v>0.05069361860261681</v>
       </c>
       <c r="M90">
-        <v>361.1788212859374</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13">
+        <v>0.05069238163197577</v>
+      </c>
+      <c r="N90">
+        <v>361.1788212859411</v>
+      </c>
+      <c r="O90">
+        <v>1.236970641041904E-06</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91">
-        <v>122.5649654055747</v>
+        <v>122.5649654055746</v>
       </c>
       <c r="B91">
-        <v>2797606.40596689</v>
+        <v>2797606.405966826</v>
       </c>
       <c r="C91">
-        <v>5010.681518019654</v>
+        <v>5010.68151801937</v>
       </c>
       <c r="D91">
-        <v>17564.13652368391</v>
+        <v>17564.13652368384</v>
       </c>
       <c r="E91">
-        <v>2348.168565198246</v>
+        <v>2348.168565198313</v>
       </c>
       <c r="F91">
-        <v>1949.119516054869</v>
+        <v>1949.119516054914</v>
       </c>
       <c r="G91">
-        <v>5.457865924548258</v>
+        <v>5.457865924548261</v>
       </c>
       <c r="H91">
-        <v>88.75047689173161</v>
+        <v>88.750476891734</v>
       </c>
       <c r="I91">
-        <v>7.467782918931125E-08</v>
+        <v>7.467782918931447E-08</v>
       </c>
       <c r="J91">
-        <v>1.640440703783255E-08</v>
+        <v>1.640440703783267E-08</v>
       </c>
       <c r="K91">
-        <v>3.738002256223593E-05</v>
+        <v>3.738002256223563E-05</v>
       </c>
       <c r="L91">
-        <v>0.04939412892799065</v>
+        <v>0.04939412892799039</v>
       </c>
       <c r="M91">
-        <v>349.5639036108689</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13">
+        <v>0.04939286433420979</v>
+      </c>
+      <c r="N91">
+        <v>349.5639036108656</v>
+      </c>
+      <c r="O91">
+        <v>1.264593780595639E-06</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92">
         <v>123.466450905875</v>
       </c>
       <c r="B92">
-        <v>2920600.246486377</v>
+        <v>2920600.246486294</v>
       </c>
       <c r="C92">
-        <v>5339.688397198038</v>
+        <v>5339.688397197584</v>
       </c>
       <c r="D92">
-        <v>17219.51728672935</v>
+        <v>17219.5172867292</v>
       </c>
       <c r="E92">
-        <v>2210.268671230142</v>
+        <v>2210.268671230244</v>
       </c>
       <c r="F92">
-        <v>1832.917748720752</v>
+        <v>1832.917748720819</v>
       </c>
       <c r="G92">
-        <v>5.477696995386857</v>
+        <v>5.477696995386943</v>
       </c>
       <c r="H92">
-        <v>96.78739379323765</v>
+        <v>96.78739379324458</v>
       </c>
       <c r="I92">
-        <v>8.70817835582979E-08</v>
+        <v>8.708178355830699E-08</v>
       </c>
       <c r="J92">
-        <v>1.710372330289232E-08</v>
+        <v>1.710372330289257E-08</v>
       </c>
       <c r="K92">
-        <v>3.598039085357071E-05</v>
+        <v>3.59803908535701E-05</v>
       </c>
       <c r="L92">
-        <v>0.04810859772644383</v>
+        <v>0.04810859772644333</v>
       </c>
       <c r="M92">
-        <v>337.7711400657758</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13">
+        <v>0.04810730485723978</v>
+      </c>
+      <c r="N92">
+        <v>337.7711400657683</v>
+      </c>
+      <c r="O92">
+        <v>1.292869203553706E-06</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
       <c r="A93">
         <v>124.3679364061753</v>
       </c>
       <c r="B93">
-        <v>3047413.434104568</v>
+        <v>3047413.434104622</v>
       </c>
       <c r="C93">
-        <v>5692.819059224282</v>
+        <v>5692.81905922458</v>
       </c>
       <c r="D93">
-        <v>16857.94471391715</v>
+        <v>16857.94471391726</v>
       </c>
       <c r="E93">
-        <v>2065.926942543351</v>
+        <v>2065.926942543302</v>
       </c>
       <c r="F93">
-        <v>1711.388781927639</v>
+        <v>1711.388781927611</v>
       </c>
       <c r="G93">
-        <v>5.506732724513329</v>
+        <v>5.506732724513268</v>
       </c>
       <c r="H93">
-        <v>106.7708303691791</v>
+        <v>106.7708303691741</v>
       </c>
       <c r="I93">
-        <v>1.030901429677413E-07</v>
+        <v>1.030901429677339E-07</v>
       </c>
       <c r="J93">
-        <v>1.785864958985836E-08</v>
+        <v>1.785864958985816E-08</v>
       </c>
       <c r="K93">
-        <v>3.458233640171353E-05</v>
+        <v>3.458233640171396E-05</v>
       </c>
       <c r="L93">
-        <v>0.04683459527537916</v>
+        <v>0.0468345952753795</v>
       </c>
       <c r="M93">
-        <v>325.7746305619381</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13">
+        <v>0.04683327342648166</v>
+      </c>
+      <c r="N93">
+        <v>325.7746305619432</v>
+      </c>
+      <c r="O93">
+        <v>1.321848897838095E-06</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
       <c r="A94">
         <v>125.2694219064756</v>
       </c>
       <c r="B94">
-        <v>3178018.575644713</v>
+        <v>3178018.575644744</v>
       </c>
       <c r="C94">
-        <v>6072.038415697534</v>
+        <v>6072.038415697722</v>
       </c>
       <c r="D94">
-        <v>16476.3580643161</v>
+        <v>16476.35806431618</v>
       </c>
       <c r="E94">
-        <v>1914.556577622637</v>
+        <v>1914.556577622597</v>
       </c>
       <c r="F94">
-        <v>1584.054354005203</v>
+        <v>1584.054354005174</v>
       </c>
       <c r="G94">
-        <v>5.54639864483432</v>
+        <v>5.546398644834289</v>
       </c>
       <c r="H94">
-        <v>119.5377359687415</v>
+        <v>119.5377359687377</v>
       </c>
       <c r="I94">
-        <v>1.243822331631934E-07</v>
+        <v>1.243822331631873E-07</v>
       </c>
       <c r="J94">
-        <v>1.867961470012699E-08</v>
+        <v>1.867961470012685E-08</v>
       </c>
       <c r="K94">
-        <v>3.318047583998238E-05</v>
+        <v>3.318047583998266E-05</v>
       </c>
       <c r="L94">
-        <v>0.04556774798139183</v>
+        <v>0.04556774798139208</v>
       </c>
       <c r="M94">
-        <v>313.5391669348278</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13">
+        <v>0.04556639637551602</v>
+      </c>
+      <c r="N94">
+        <v>313.5391669348309</v>
+      </c>
+      <c r="O94">
+        <v>1.351605876063198E-06</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95">
         <v>126.1709074067759</v>
       </c>
       <c r="B95">
-        <v>3312357.038763612</v>
+        <v>3312357.038763616</v>
       </c>
       <c r="C95">
-        <v>6480.24982010996</v>
+        <v>6480.249820109987</v>
       </c>
       <c r="D95">
-        <v>16070.45641357385</v>
+        <v>16070.45641357382</v>
       </c>
       <c r="E95">
-        <v>1755.154571126853</v>
+        <v>1755.154571126841</v>
       </c>
       <c r="F95">
-        <v>1450.122750995409</v>
+        <v>1450.122750995396</v>
       </c>
       <c r="G95">
-        <v>5.598572726198873</v>
+        <v>5.598572726198891</v>
       </c>
       <c r="H95">
-        <v>136.4835315804056</v>
+        <v>136.4835315804087</v>
       </c>
       <c r="I95">
-        <v>1.538241807499452E-07</v>
+        <v>1.538241807499501E-07</v>
       </c>
       <c r="J95">
-        <v>1.958108894232646E-08</v>
+        <v>1.958108894232653E-08</v>
       </c>
       <c r="K95">
-        <v>3.176708494394925E-05</v>
+        <v>3.176708494394913E-05</v>
       </c>
       <c r="L95">
-        <v>0.04430091521062589</v>
+        <v>0.04430091521062579</v>
       </c>
       <c r="M95">
-        <v>301.0153900515022</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13">
+        <v>0.04429953296412593</v>
+      </c>
+      <c r="N95">
+        <v>301.0153900515004</v>
+      </c>
+      <c r="O95">
+        <v>1.382246499862264E-06</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96">
         <v>127.0723929070762</v>
       </c>
       <c r="B96">
-        <v>3450340.476029715</v>
+        <v>3450340.476029635</v>
       </c>
       <c r="C96">
-        <v>6922.21210311338</v>
+        <v>6922.212103112787</v>
       </c>
       <c r="D96">
-        <v>15633.91732928174</v>
+        <v>15633.91732928162</v>
       </c>
       <c r="E96">
-        <v>1585.974940187123</v>
+        <v>1585.974940187228</v>
       </c>
       <c r="F96">
-        <v>1308.225999387648</v>
+        <v>1308.22599938772</v>
       </c>
       <c r="G96">
-        <v>5.665857345460514</v>
+        <v>5.665857345460581</v>
       </c>
       <c r="H96">
-        <v>160.1207327403522</v>
+        <v>160.1207327403678</v>
       </c>
       <c r="I96">
-        <v>1.967095461190746E-07</v>
+        <v>1.967095461190991E-07</v>
       </c>
       <c r="J96">
-        <v>2.058416303441283E-08</v>
+        <v>2.058416303441308E-08</v>
       </c>
       <c r="K96">
-        <v>3.03306013023954E-05</v>
+        <v>3.0330601302395E-05</v>
       </c>
       <c r="L96">
-        <v>0.04302277659009134</v>
+        <v>0.04302277659009103</v>
       </c>
       <c r="M96">
-        <v>288.131334390136</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13">
+        <v>0.04302136265801547</v>
+      </c>
+      <c r="N96">
+        <v>288.1313343901306</v>
+      </c>
+      <c r="O96">
+        <v>1.41393207555955E-06</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97">
         <v>127.9738784073765</v>
       </c>
       <c r="B97">
-        <v>3591855.067192324</v>
+        <v>3591855.067192333</v>
       </c>
       <c r="C97">
-        <v>7406.23294958776</v>
+        <v>7406.232949587881</v>
       </c>
       <c r="D97">
-        <v>15156.86356608863</v>
+        <v>15156.86356608875</v>
       </c>
       <c r="E97">
-        <v>1403.939336781118</v>
+        <v>1403.939336781119</v>
       </c>
       <c r="F97">
-        <v>1155.940790702845</v>
+        <v>1155.940790702852</v>
       </c>
       <c r="G97">
-        <v>5.752099158004547</v>
+        <v>5.752099158004487</v>
       </c>
       <c r="H97">
-        <v>195.4757684141885</v>
+        <v>195.4757684141725</v>
       </c>
       <c r="I97">
-        <v>2.639284056003044E-07</v>
+        <v>2.63928405600276E-07</v>
       </c>
       <c r="J97">
-        <v>2.172164869567559E-08</v>
+        <v>2.172164869567533E-08</v>
       </c>
       <c r="K97">
-        <v>2.885271714973035E-05</v>
+        <v>2.88527171497307E-05</v>
       </c>
       <c r="L97">
-        <v>0.04171514142299483</v>
+        <v>0.04171514142299512</v>
       </c>
       <c r="M97">
-        <v>274.7760339623196</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13">
+        <v>0.04171369450233498</v>
+      </c>
+      <c r="N97">
+        <v>274.7760339623238</v>
+      </c>
+      <c r="O97">
+        <v>1.446920660136919E-06</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98">
         <v>128.8753639076768</v>
       </c>
       <c r="B98">
-        <v>3736767.779351325</v>
+        <v>3736767.779351403</v>
       </c>
       <c r="C98">
-        <v>7947.749301460408</v>
+        <v>7947.749301461314</v>
       </c>
       <c r="D98">
-        <v>14622.42944601264</v>
+        <v>14622.42944601311</v>
       </c>
       <c r="E98">
-        <v>1203.387289878965</v>
+        <v>1203.387289878847</v>
       </c>
       <c r="F98">
-        <v>988.77090540043</v>
+        <v>988.7709054003523</v>
       </c>
       <c r="G98">
-        <v>5.863516695809752</v>
+        <v>5.863516695809531</v>
       </c>
       <c r="H98">
-        <v>254.2803412951873</v>
+        <v>254.2803412950859</v>
       </c>
       <c r="I98">
-        <v>3.817048440554897E-07</v>
+        <v>3.817048440552984E-07</v>
       </c>
       <c r="J98">
-        <v>2.304957510992058E-08</v>
+        <v>2.304957510991947E-08</v>
       </c>
       <c r="K98">
-        <v>2.730189324492916E-05</v>
+        <v>2.730189324493056E-05</v>
       </c>
       <c r="L98">
-        <v>0.04034709327579758</v>
+        <v>0.04034709327579863</v>
       </c>
       <c r="M98">
-        <v>260.7628841619662</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13">
+        <v>0.04034561161580106</v>
+      </c>
+      <c r="N98">
+        <v>260.7628841619817</v>
+      </c>
+      <c r="O98">
+        <v>1.481659997567688E-06</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99">
         <v>129.7768494079772</v>
       </c>
       <c r="B99">
-        <v>3884933.58353242</v>
+        <v>3884933.583532443</v>
       </c>
       <c r="C99">
-        <v>8578.828321721692</v>
+        <v>8578.82832172228</v>
       </c>
       <c r="D99">
-        <v>13997.36463213533</v>
+        <v>13997.36463213572</v>
       </c>
       <c r="E99">
-        <v>972.7274308941869</v>
+        <v>972.7274308941353</v>
       </c>
       <c r="F99">
-        <v>797.4236295794798</v>
+        <v>797.4236295794476</v>
       </c>
       <c r="G99">
-        <v>6.011674717911373</v>
+        <v>6.011674717911205</v>
       </c>
       <c r="H99">
-        <v>371.7403749603058</v>
+        <v>371.7403749601638</v>
       </c>
       <c r="I99">
-        <v>6.316433381036757E-07</v>
+        <v>6.316433381033808E-07</v>
       </c>
       <c r="J99">
-        <v>2.467884292750135E-08</v>
+        <v>2.467884292750035E-08</v>
       </c>
       <c r="K99">
-        <v>2.56156011231653E-05</v>
+        <v>2.561560112316636E-05</v>
       </c>
       <c r="L99">
-        <v>0.03885945130734215</v>
+        <v>0.03885945130734295</v>
       </c>
       <c r="M99">
-        <v>245.7289545727166</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13">
+        <v>0.03885793226608245</v>
+      </c>
+      <c r="N99">
+        <v>245.7289545727278</v>
+      </c>
+      <c r="O99">
+        <v>1.519041260499948E-06</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
       <c r="A100">
         <v>130.6783349082775</v>
       </c>
       <c r="B100">
-        <v>4036202.563376951</v>
+        <v>4036202.563376758</v>
       </c>
       <c r="C100">
-        <v>9385.155784175955</v>
+        <v>9385.155784170498</v>
       </c>
       <c r="D100">
-        <v>13195.09763078931</v>
+        <v>13195.09763078589</v>
       </c>
       <c r="E100">
-        <v>681.3167250140895</v>
+        <v>681.3167250145915</v>
       </c>
       <c r="F100">
-        <v>557.1408563010581</v>
+        <v>557.1408563013958</v>
       </c>
       <c r="G100">
-        <v>6.224679908133219</v>
+        <v>6.22467990813476</v>
       </c>
       <c r="H100">
-        <v>723.908466045265</v>
+        <v>723.9084660491736</v>
       </c>
       <c r="I100">
-        <v>1.441240174596116E-06</v>
+        <v>1.441240174604924E-06</v>
       </c>
       <c r="J100">
-        <v>2.690051854127674E-08</v>
+        <v>2.690051854128599E-08</v>
       </c>
       <c r="K100">
-        <v>2.363033581740252E-05</v>
+        <v>2.363033581739419E-05</v>
       </c>
       <c r="L100">
-        <v>0.03710550550289189</v>
+        <v>0.0371055055028856</v>
       </c>
       <c r="M100">
-        <v>228.7362270479292</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13">
+        <v>0.03710394410518936</v>
+      </c>
+      <c r="N100">
+        <v>228.736227047847</v>
+      </c>
+      <c r="O100">
+        <v>1.561397696243383E-06</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
       <c r="A101">
         <v>131.5798204085778</v>
       </c>
       <c r="B101">
-        <v>4190425.254551645</v>
+        <v>4190425.252084599</v>
       </c>
       <c r="C101">
-        <v>11329.48695083199</v>
+        <v>11330.07281506585</v>
       </c>
       <c r="D101">
-        <v>11335.73244277654</v>
+        <v>11335.1726221328</v>
       </c>
       <c r="E101">
-        <v>1.111278950427252</v>
+        <v>0.9074233820926141</v>
       </c>
       <c r="F101">
-        <v>0.9074973727085082</v>
+        <v>0.7410242698033497</v>
       </c>
       <c r="G101">
-        <v>6.753716347044994</v>
+        <v>6.753870040806118</v>
       </c>
       <c r="H101">
-        <v>6354497.687883534</v>
+        <v>7814667.297611522</v>
       </c>
       <c r="I101">
-        <v>0.01813470541920055</v>
+        <v>0.02230416219273524</v>
       </c>
       <c r="J101">
-        <v>3.273060151844122E-08</v>
+        <v>3.273252747442864E-08</v>
       </c>
       <c r="K101">
-        <v>1.967031536392637E-05</v>
+        <v>1.966923883540698E-05</v>
       </c>
       <c r="L101">
-        <v>0.03368382224194097</v>
+        <v>0.03368293329520157</v>
       </c>
       <c r="M101">
-        <v>200.1512653642017</v>
+        <v>0.03368130062078444</v>
+      </c>
+      <c r="N101">
+        <v>200.1449311367725</v>
+      </c>
+      <c r="O101">
+        <v>1.632674417136799E-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>